<commit_message>
añdir subneteo de sucursal Walmart
</commit_message>
<xml_diff>
--- a/SUBNETEO REDES.xlsx
+++ b/SUBNETEO REDES.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Documents\Universidad\Redes II\TERCER PARCIAL\Proyecto\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Documents\Universidad\Redes II\TERCER PARCIAL\Proyecto\PROYECTO-REDES\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -13,10 +13,9 @@
   </bookViews>
   <sheets>
     <sheet name="Resumen" sheetId="1" r:id="rId1"/>
-    <sheet name="Hoja1" sheetId="7" r:id="rId2"/>
-    <sheet name="Info.General" sheetId="2" r:id="rId3"/>
-    <sheet name="VLANS" sheetId="6" r:id="rId4"/>
-    <sheet name="Honduras" sheetId="5" state="hidden" r:id="rId5"/>
+    <sheet name="Info.General" sheetId="2" r:id="rId2"/>
+    <sheet name="VLANS" sheetId="6" r:id="rId3"/>
+    <sheet name="Honduras" sheetId="5" state="hidden" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="973" uniqueCount="290">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1167" uniqueCount="396">
   <si>
     <t>REDES:5</t>
   </si>
@@ -744,24 +743,9 @@
     <t>255.255.255.252/21</t>
   </si>
   <si>
-    <t>172.168.0.1 - 172.168.0.254</t>
-  </si>
-  <si>
-    <t>172.168.1.1 - 172.168.1.254</t>
-  </si>
-  <si>
-    <t>172.168.2.1 - 172.168.2.254</t>
-  </si>
-  <si>
-    <t>4 4</t>
-  </si>
-  <si>
     <t>172.168.3.0</t>
   </si>
   <si>
-    <t>172.168.3.1 - 172.168.3.254</t>
-  </si>
-  <si>
     <t>172.168.33.0</t>
   </si>
   <si>
@@ -898,6 +882,339 @@
   </si>
   <si>
     <t>Sub red oficinas</t>
+  </si>
+  <si>
+    <t>/27</t>
+  </si>
+  <si>
+    <t>172.168.24.31</t>
+  </si>
+  <si>
+    <t>172.168.24.32</t>
+  </si>
+  <si>
+    <t>172.168.24.63</t>
+  </si>
+  <si>
+    <t>DIRECCION GENERAL</t>
+  </si>
+  <si>
+    <t>172.168.24.64</t>
+  </si>
+  <si>
+    <t>172.168.24.95</t>
+  </si>
+  <si>
+    <t>172.168.24.96</t>
+  </si>
+  <si>
+    <t>172.168.24.127</t>
+  </si>
+  <si>
+    <t>172.168.24.128</t>
+  </si>
+  <si>
+    <t>172.168.24.159</t>
+  </si>
+  <si>
+    <t>172.168.24.160</t>
+  </si>
+  <si>
+    <t>172.168.24.191</t>
+  </si>
+  <si>
+    <t>172.168.24.192</t>
+  </si>
+  <si>
+    <t>172.168.24.223</t>
+  </si>
+  <si>
+    <t>172.168.24.30</t>
+  </si>
+  <si>
+    <t>172.168.24.62</t>
+  </si>
+  <si>
+    <t>172.168.24.94</t>
+  </si>
+  <si>
+    <t>172.168.24.126</t>
+  </si>
+  <si>
+    <t>172.168.24.158</t>
+  </si>
+  <si>
+    <t>172.168.24.190</t>
+  </si>
+  <si>
+    <t>172.168.24.222</t>
+  </si>
+  <si>
+    <t>172.168.24.1</t>
+  </si>
+  <si>
+    <t>172.168.24.33</t>
+  </si>
+  <si>
+    <t xml:space="preserve">172.168.24.65 </t>
+  </si>
+  <si>
+    <t>172.168.24.97</t>
+  </si>
+  <si>
+    <t>172.168.24.129</t>
+  </si>
+  <si>
+    <t xml:space="preserve">172.168.24.161 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">172.168.24.193 </t>
+  </si>
+  <si>
+    <t>Sub Red MASXMENOS</t>
+  </si>
+  <si>
+    <t>172.168.28.0</t>
+  </si>
+  <si>
+    <t>172.168.26.31</t>
+  </si>
+  <si>
+    <t>172.168.26.32</t>
+  </si>
+  <si>
+    <t>172.168.26.63</t>
+  </si>
+  <si>
+    <t>172.168.26.64</t>
+  </si>
+  <si>
+    <t>172.168.26.95</t>
+  </si>
+  <si>
+    <t>172.168.26.96</t>
+  </si>
+  <si>
+    <t>172.168.26.127</t>
+  </si>
+  <si>
+    <t>172.168.26.128</t>
+  </si>
+  <si>
+    <t>172.168.26.159</t>
+  </si>
+  <si>
+    <t>172.168.26.160</t>
+  </si>
+  <si>
+    <t>172.168.26.191</t>
+  </si>
+  <si>
+    <t>172.168.26.192</t>
+  </si>
+  <si>
+    <t>172.168.26.223</t>
+  </si>
+  <si>
+    <t>172.168.26.30</t>
+  </si>
+  <si>
+    <t>172.168.26.62</t>
+  </si>
+  <si>
+    <t>172.168.26.94</t>
+  </si>
+  <si>
+    <t>172.168.26.126</t>
+  </si>
+  <si>
+    <t>172.168.26.158</t>
+  </si>
+  <si>
+    <t>172.168.26.190</t>
+  </si>
+  <si>
+    <t>172.168.26.222</t>
+  </si>
+  <si>
+    <t xml:space="preserve">172.168.26.33 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">172.168.26.65 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">172.168.26.97 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">172.168.26.129 </t>
+  </si>
+  <si>
+    <t>172.168.26.161</t>
+  </si>
+  <si>
+    <t xml:space="preserve">172.168.26.193 </t>
+  </si>
+  <si>
+    <t>Sub Red PALI</t>
+  </si>
+  <si>
+    <t>172.168.27.31</t>
+  </si>
+  <si>
+    <t>172.168.27.32</t>
+  </si>
+  <si>
+    <t>172.168.27.63</t>
+  </si>
+  <si>
+    <t>172.168.27.64</t>
+  </si>
+  <si>
+    <t>172.168.27.95</t>
+  </si>
+  <si>
+    <t>172.168.27.96</t>
+  </si>
+  <si>
+    <t>172.168.27.127</t>
+  </si>
+  <si>
+    <t>172.168.27.128</t>
+  </si>
+  <si>
+    <t>172.168.27.159</t>
+  </si>
+  <si>
+    <t>172.168.27.160</t>
+  </si>
+  <si>
+    <t>172.168.27.191</t>
+  </si>
+  <si>
+    <t>172.168.27.192</t>
+  </si>
+  <si>
+    <t>172.168.27.223</t>
+  </si>
+  <si>
+    <t>172.168.27.30</t>
+  </si>
+  <si>
+    <t>172.168.27.62</t>
+  </si>
+  <si>
+    <t>172.168.27.94</t>
+  </si>
+  <si>
+    <t>172.168.27.126</t>
+  </si>
+  <si>
+    <t>172.168.27.158</t>
+  </si>
+  <si>
+    <t>172.168.27.190</t>
+  </si>
+  <si>
+    <t>172.168.27.222</t>
+  </si>
+  <si>
+    <t>172.168.27.33</t>
+  </si>
+  <si>
+    <t xml:space="preserve">172.168.27.65 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">172.168.27.97 </t>
+  </si>
+  <si>
+    <t>172.168.27.129</t>
+  </si>
+  <si>
+    <t xml:space="preserve">172.168.27.161 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">172.168.27.193 </t>
+  </si>
+  <si>
+    <t>Sub Red MAXIPALI</t>
+  </si>
+  <si>
+    <t>172.168.28.31</t>
+  </si>
+  <si>
+    <t>172.168.28.32</t>
+  </si>
+  <si>
+    <t>172.168.28.63</t>
+  </si>
+  <si>
+    <t>172.168.28.64</t>
+  </si>
+  <si>
+    <t>172.168.28.95</t>
+  </si>
+  <si>
+    <t>172.168.28.96</t>
+  </si>
+  <si>
+    <t>172.168.28.127</t>
+  </si>
+  <si>
+    <t>172.168.28.128</t>
+  </si>
+  <si>
+    <t>172.168.28.159</t>
+  </si>
+  <si>
+    <t>172.168.28.160</t>
+  </si>
+  <si>
+    <t>172.168.28.191</t>
+  </si>
+  <si>
+    <t>172.168.28.192</t>
+  </si>
+  <si>
+    <t>/28</t>
+  </si>
+  <si>
+    <t>255.255.255.240</t>
+  </si>
+  <si>
+    <t>172.168.28.223</t>
+  </si>
+  <si>
+    <t>172.168.28.30</t>
+  </si>
+  <si>
+    <t>172.168.28.65</t>
+  </si>
+  <si>
+    <t>172.168.28.66</t>
+  </si>
+  <si>
+    <t>172.168.28.67</t>
+  </si>
+  <si>
+    <t>172.168.28.62</t>
+  </si>
+  <si>
+    <t xml:space="preserve">172.168.28.33 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">172.168.28.65 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">172.168.28.97 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">172.168.28.129 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">172.168.28.161 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">172.168.28.193 </t>
   </si>
 </sst>
 </file>
@@ -929,7 +1246,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -980,13 +1297,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.59999389629810485"/>
+        <fgColor theme="9" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="-0.249977111117893"/>
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1172,7 +1495,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="91">
+  <cellXfs count="99">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -1286,33 +1609,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1334,28 +1630,71 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1644,10 +1983,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AW111"/>
+  <dimension ref="A1:AX111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AH21" workbookViewId="0">
-      <selection activeCell="AL42" sqref="AL42"/>
+    <sheetView tabSelected="1" topLeftCell="AI73" workbookViewId="0">
+      <selection activeCell="AU91" sqref="AU91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1693,7 +2032,7 @@
     <col min="45" max="45" width="9.85546875" customWidth="1"/>
     <col min="46" max="46" width="14.42578125" customWidth="1"/>
     <col min="47" max="47" width="15.5703125" customWidth="1"/>
-    <col min="48" max="48" width="13.7109375" customWidth="1"/>
+    <col min="48" max="48" width="15.42578125" customWidth="1"/>
     <col min="49" max="49" width="13.85546875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2292,10 +2631,10 @@
         <v>236</v>
       </c>
       <c r="H25" s="37" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="I25" s="40" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="J25" s="6"/>
       <c r="K25" s="33" t="s">
@@ -2424,16 +2763,16 @@
         <v>116</v>
       </c>
       <c r="F26" s="37" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
       <c r="G26" s="37" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="H26" s="37" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="I26" s="40" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="J26" s="6"/>
       <c r="K26" s="33" t="s">
@@ -2527,7 +2866,7 @@
         <v>254</v>
       </c>
       <c r="AR26" s="37" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="AS26" s="37" t="s">
         <v>231</v>
@@ -2539,10 +2878,10 @@
         <v>235</v>
       </c>
       <c r="AV26" s="37" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="AW26" s="37" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
     </row>
     <row r="27" spans="1:49" x14ac:dyDescent="0.25">
@@ -2562,16 +2901,16 @@
         <v>116</v>
       </c>
       <c r="F27" s="37" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
       <c r="G27" s="37" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="H27" s="37" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="I27" s="40" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="J27" s="6"/>
       <c r="K27" s="33" t="s">
@@ -2656,7 +2995,7 @@
         <v>120</v>
       </c>
       <c r="AO27" s="33" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
       <c r="AP27" s="37">
         <v>152</v>
@@ -2671,16 +3010,16 @@
         <v>116</v>
       </c>
       <c r="AT27" s="37" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="AU27" s="37" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="AV27" s="37" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="AW27" s="37" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
     </row>
     <row r="28" spans="1:49" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2700,16 +3039,16 @@
         <v>116</v>
       </c>
       <c r="F28" s="38" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="G28" s="61" t="s">
+        <v>243</v>
+      </c>
+      <c r="H28" s="38" t="s">
         <v>248</v>
       </c>
-      <c r="H28" s="38" t="s">
-        <v>253</v>
-      </c>
       <c r="I28" s="41" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="J28" s="6"/>
       <c r="K28" s="34" t="s">
@@ -2728,7 +3067,7 @@
         <v>116</v>
       </c>
       <c r="P28" s="38" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="Q28" s="38" t="s">
         <v>144</v>
@@ -2809,16 +3148,16 @@
         <v>116</v>
       </c>
       <c r="AT28" s="37" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="AU28" s="37" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="AV28" s="37" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="AW28" s="37" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
     </row>
     <row r="29" spans="1:49" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2897,16 +3236,16 @@
         <v>116</v>
       </c>
       <c r="AT29" s="38" t="s">
-        <v>260</v>
+        <v>315</v>
       </c>
       <c r="AU29" s="38" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="AV29" s="38" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="AW29" s="38" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
     </row>
     <row r="30" spans="1:49" x14ac:dyDescent="0.25">
@@ -2918,8 +3257,8 @@
     <row r="31" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A31" s="32"/>
       <c r="AN31" s="62"/>
-      <c r="AO31" s="60" t="s">
-        <v>275</v>
+      <c r="AO31" s="89" t="s">
+        <v>270</v>
       </c>
       <c r="AR31" s="62"/>
       <c r="AS31" s="62"/>
@@ -2959,7 +3298,7 @@
         <v>103</v>
       </c>
       <c r="AP34" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="AQ34" t="s">
         <v>231</v>
@@ -2976,31 +3315,31 @@
       <c r="H35" s="44"/>
       <c r="I35" s="45"/>
       <c r="AN35" s="62"/>
-      <c r="AO35" s="72" t="s">
+      <c r="AO35" s="63" t="s">
         <v>94</v>
       </c>
-      <c r="AP35" s="73" t="s">
+      <c r="AP35" s="64" t="s">
         <v>95</v>
       </c>
-      <c r="AQ35" s="73" t="s">
+      <c r="AQ35" s="64" t="s">
         <v>96</v>
       </c>
-      <c r="AR35" s="73" t="s">
+      <c r="AR35" s="64" t="s">
         <v>103</v>
       </c>
-      <c r="AS35" s="73" t="s">
+      <c r="AS35" s="64" t="s">
         <v>102</v>
       </c>
-      <c r="AT35" s="73" t="s">
+      <c r="AT35" s="64" t="s">
         <v>104</v>
       </c>
-      <c r="AU35" s="73" t="s">
+      <c r="AU35" s="64" t="s">
         <v>101</v>
       </c>
-      <c r="AV35" s="73" t="s">
+      <c r="AV35" s="64" t="s">
         <v>43</v>
       </c>
-      <c r="AW35" s="74" t="s">
+      <c r="AW35" s="65" t="s">
         <v>40</v>
       </c>
     </row>
@@ -3015,32 +3354,32 @@
       <c r="H36" s="42"/>
       <c r="I36" s="42"/>
       <c r="AN36" s="62"/>
-      <c r="AO36" s="75" t="s">
-        <v>277</v>
-      </c>
-      <c r="AP36" s="76">
+      <c r="AO36" s="66" t="s">
+        <v>272</v>
+      </c>
+      <c r="AP36" s="67">
         <v>143</v>
       </c>
-      <c r="AQ36" s="76">
+      <c r="AQ36" s="67">
         <v>254</v>
       </c>
-      <c r="AR36" s="76" t="s">
+      <c r="AR36" s="67" t="s">
         <v>117</v>
       </c>
-      <c r="AS36" s="76" t="s">
+      <c r="AS36" s="67" t="s">
         <v>116</v>
       </c>
-      <c r="AT36" s="76" t="s">
+      <c r="AT36" s="67" t="s">
         <v>232</v>
       </c>
-      <c r="AU36" s="76" t="s">
+      <c r="AU36" s="67" t="s">
         <v>235</v>
       </c>
-      <c r="AV36" s="76" t="s">
-        <v>263</v>
-      </c>
-      <c r="AW36" s="77" t="s">
-        <v>267</v>
+      <c r="AV36" s="67" t="s">
+        <v>258</v>
+      </c>
+      <c r="AW36" s="68" t="s">
+        <v>262</v>
       </c>
     </row>
     <row r="37" spans="1:49" x14ac:dyDescent="0.25">
@@ -3053,32 +3392,32 @@
       <c r="G37" s="42"/>
       <c r="H37" s="42"/>
       <c r="I37" s="42"/>
-      <c r="AO37" s="75" t="s">
-        <v>278</v>
-      </c>
-      <c r="AP37" s="76">
+      <c r="AO37" s="66" t="s">
+        <v>273</v>
+      </c>
+      <c r="AP37" s="67">
         <v>50</v>
       </c>
-      <c r="AQ37" s="76">
+      <c r="AQ37" s="67">
         <v>62</v>
       </c>
-      <c r="AR37" s="76" t="s">
+      <c r="AR37" s="67" t="s">
+        <v>275</v>
+      </c>
+      <c r="AS37" s="67" t="s">
+        <v>274</v>
+      </c>
+      <c r="AT37" s="67" t="s">
+        <v>253</v>
+      </c>
+      <c r="AU37" s="67" t="s">
+        <v>282</v>
+      </c>
+      <c r="AV37" s="67" t="s">
         <v>280</v>
       </c>
-      <c r="AS37" s="76" t="s">
-        <v>279</v>
-      </c>
-      <c r="AT37" s="76" t="s">
-        <v>258</v>
-      </c>
-      <c r="AU37" s="76" t="s">
-        <v>287</v>
-      </c>
-      <c r="AV37" s="76" t="s">
-        <v>285</v>
-      </c>
-      <c r="AW37" s="77" t="s">
-        <v>281</v>
+      <c r="AW37" s="68" t="s">
+        <v>276</v>
       </c>
     </row>
     <row r="38" spans="1:49" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3091,33 +3430,33 @@
       <c r="G38" s="42"/>
       <c r="H38" s="42"/>
       <c r="I38" s="42"/>
-      <c r="AN38" s="90"/>
-      <c r="AO38" s="78" t="s">
-        <v>282</v>
-      </c>
-      <c r="AP38" s="79">
+      <c r="AN38" s="75"/>
+      <c r="AO38" s="69" t="s">
+        <v>277</v>
+      </c>
+      <c r="AP38" s="70">
         <v>50</v>
       </c>
-      <c r="AQ38" s="79">
+      <c r="AQ38" s="70">
         <v>62</v>
       </c>
-      <c r="AR38" s="79" t="s">
-        <v>280</v>
-      </c>
-      <c r="AS38" s="79" t="s">
+      <c r="AR38" s="70" t="s">
+        <v>275</v>
+      </c>
+      <c r="AS38" s="70" t="s">
+        <v>274</v>
+      </c>
+      <c r="AT38" s="70" t="s">
+        <v>278</v>
+      </c>
+      <c r="AU38" s="70" t="s">
+        <v>283</v>
+      </c>
+      <c r="AV38" s="70" t="s">
+        <v>281</v>
+      </c>
+      <c r="AW38" s="71" t="s">
         <v>279</v>
-      </c>
-      <c r="AT38" s="79" t="s">
-        <v>283</v>
-      </c>
-      <c r="AU38" s="79" t="s">
-        <v>288</v>
-      </c>
-      <c r="AV38" s="79" t="s">
-        <v>286</v>
-      </c>
-      <c r="AW38" s="80" t="s">
-        <v>284</v>
       </c>
     </row>
     <row r="39" spans="1:49" x14ac:dyDescent="0.25">
@@ -3150,7 +3489,7 @@
       <c r="H40" s="42"/>
       <c r="I40" s="42"/>
       <c r="AO40" s="60" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
     </row>
     <row r="41" spans="1:49" x14ac:dyDescent="0.25">
@@ -3205,136 +3544,250 @@
       </c>
     </row>
     <row r="44" spans="1:49" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="AO44" s="87" t="s">
+      <c r="AO44" s="72" t="s">
         <v>94</v>
       </c>
-      <c r="AP44" s="88" t="s">
+      <c r="AP44" s="73" t="s">
         <v>95</v>
       </c>
-      <c r="AQ44" s="88" t="s">
+      <c r="AQ44" s="73" t="s">
         <v>96</v>
       </c>
-      <c r="AR44" s="88" t="s">
+      <c r="AR44" s="73" t="s">
         <v>103</v>
       </c>
-      <c r="AS44" s="88" t="s">
+      <c r="AS44" s="73" t="s">
         <v>102</v>
       </c>
-      <c r="AT44" s="88" t="s">
+      <c r="AT44" s="73" t="s">
         <v>104</v>
       </c>
-      <c r="AU44" s="88" t="s">
+      <c r="AU44" s="73" t="s">
         <v>101</v>
       </c>
-      <c r="AV44" s="88" t="s">
+      <c r="AV44" s="73" t="s">
         <v>43</v>
       </c>
-      <c r="AW44" s="89" t="s">
+      <c r="AW44" s="74" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="45" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="AO45" s="81" t="s">
-        <v>277</v>
-      </c>
-      <c r="AP45" s="82">
-        <v>143</v>
-      </c>
-      <c r="AQ45" s="82">
-        <v>254</v>
-      </c>
-      <c r="AR45" s="82" t="s">
-        <v>117</v>
-      </c>
-      <c r="AS45" s="82" t="s">
-        <v>116</v>
-      </c>
-      <c r="AT45" s="82" t="s">
+      <c r="AO45" s="85" t="s">
+        <v>151</v>
+      </c>
+      <c r="AP45" s="86">
+        <v>23</v>
+      </c>
+      <c r="AQ45" s="86">
+        <v>30</v>
+      </c>
+      <c r="AR45" s="86" t="s">
+        <v>59</v>
+      </c>
+      <c r="AS45" s="86" t="s">
+        <v>285</v>
+      </c>
+      <c r="AT45" s="86" t="s">
         <v>232</v>
       </c>
-      <c r="AU45" s="82" t="s">
-        <v>235</v>
-      </c>
-      <c r="AV45" s="82" t="s">
-        <v>263</v>
-      </c>
-      <c r="AW45" s="83" t="s">
-        <v>267</v>
+      <c r="AU45" s="86" t="s">
+        <v>307</v>
+      </c>
+      <c r="AV45" s="86" t="s">
+        <v>300</v>
+      </c>
+      <c r="AW45" s="86" t="s">
+        <v>286</v>
       </c>
     </row>
     <row r="46" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="AO46" s="81" t="s">
-        <v>278</v>
-      </c>
-      <c r="AP46" s="82">
-        <v>50</v>
-      </c>
-      <c r="AQ46" s="82">
-        <v>62</v>
-      </c>
-      <c r="AR46" s="82" t="s">
-        <v>280</v>
-      </c>
-      <c r="AS46" s="82" t="s">
-        <v>279</v>
-      </c>
-      <c r="AT46" s="82" t="s">
-        <v>258</v>
-      </c>
-      <c r="AU46" s="82" t="s">
+      <c r="AO46" s="85" t="s">
+        <v>150</v>
+      </c>
+      <c r="AP46" s="86">
+        <v>22</v>
+      </c>
+      <c r="AQ46" s="86">
+        <v>30</v>
+      </c>
+      <c r="AR46" s="86" t="s">
+        <v>59</v>
+      </c>
+      <c r="AS46" s="86" t="s">
+        <v>285</v>
+      </c>
+      <c r="AT46" s="86" t="s">
         <v>287</v>
       </c>
-      <c r="AV46" s="82" t="s">
+      <c r="AU46" s="86" t="s">
+        <v>308</v>
+      </c>
+      <c r="AV46" s="86" t="s">
+        <v>301</v>
+      </c>
+      <c r="AW46" s="86" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="47" spans="1:49" x14ac:dyDescent="0.25">
+      <c r="AO47" s="85" t="s">
+        <v>289</v>
+      </c>
+      <c r="AP47" s="86">
+        <v>21</v>
+      </c>
+      <c r="AQ47" s="86">
+        <v>30</v>
+      </c>
+      <c r="AR47" s="86" t="s">
+        <v>59</v>
+      </c>
+      <c r="AS47" s="86" t="s">
         <v>285</v>
       </c>
-      <c r="AW46" s="83" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="47" spans="1:49" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="AO47" s="84" t="s">
-        <v>282</v>
-      </c>
-      <c r="AP47" s="85">
-        <v>50</v>
-      </c>
-      <c r="AQ47" s="85">
-        <v>62</v>
-      </c>
-      <c r="AR47" s="85" t="s">
-        <v>280</v>
-      </c>
-      <c r="AS47" s="85" t="s">
-        <v>279</v>
-      </c>
-      <c r="AT47" s="85" t="s">
-        <v>283</v>
-      </c>
-      <c r="AU47" s="85" t="s">
-        <v>288</v>
-      </c>
-      <c r="AV47" s="85" t="s">
-        <v>286</v>
+      <c r="AT47" s="86" t="s">
+        <v>290</v>
+      </c>
+      <c r="AU47" s="86" t="s">
+        <v>309</v>
+      </c>
+      <c r="AV47" s="86" t="s">
+        <v>302</v>
       </c>
       <c r="AW47" s="86" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="48" spans="1:49" x14ac:dyDescent="0.25">
+      <c r="AO48" s="85" t="s">
+        <v>153</v>
+      </c>
+      <c r="AP48" s="86">
+        <v>20</v>
+      </c>
+      <c r="AQ48" s="86">
+        <v>30</v>
+      </c>
+      <c r="AR48" s="86" t="s">
+        <v>59</v>
+      </c>
+      <c r="AS48" s="86" t="s">
+        <v>285</v>
+      </c>
+      <c r="AT48" s="86" t="s">
+        <v>292</v>
+      </c>
+      <c r="AU48" s="86" t="s">
+        <v>310</v>
+      </c>
+      <c r="AV48" s="86" t="s">
+        <v>303</v>
+      </c>
+      <c r="AW48" s="86" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="49" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="AO49" s="85" t="s">
+        <v>149</v>
+      </c>
+      <c r="AP49" s="86">
+        <v>20</v>
+      </c>
+      <c r="AQ49" s="86">
+        <v>30</v>
+      </c>
+      <c r="AR49" s="86" t="s">
+        <v>59</v>
+      </c>
+      <c r="AS49" s="86" t="s">
+        <v>285</v>
+      </c>
+      <c r="AT49" s="86" t="s">
+        <v>294</v>
+      </c>
+      <c r="AU49" s="86" t="s">
+        <v>311</v>
+      </c>
+      <c r="AV49" s="86" t="s">
+        <v>304</v>
+      </c>
+      <c r="AW49" s="86" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="50" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="AO50" s="85" t="s">
+        <v>154</v>
+      </c>
+      <c r="AP50" s="86">
+        <v>19</v>
+      </c>
+      <c r="AQ50" s="86">
+        <v>30</v>
+      </c>
+      <c r="AR50" s="86" t="s">
+        <v>59</v>
+      </c>
+      <c r="AS50" s="86" t="s">
+        <v>285</v>
+      </c>
+      <c r="AT50" s="86" t="s">
+        <v>296</v>
+      </c>
+      <c r="AU50" s="86" t="s">
+        <v>312</v>
+      </c>
+      <c r="AV50" s="86" t="s">
+        <v>305</v>
+      </c>
+      <c r="AW50" s="86" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="51" spans="1:50" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="28"/>
       <c r="B51" s="6"/>
       <c r="C51" s="6"/>
       <c r="D51" s="6"/>
       <c r="E51" s="6"/>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="AO51" s="87" t="s">
+        <v>152</v>
+      </c>
+      <c r="AP51" s="88">
+        <v>18</v>
+      </c>
+      <c r="AQ51" s="88">
+        <v>30</v>
+      </c>
+      <c r="AR51" s="88" t="s">
+        <v>59</v>
+      </c>
+      <c r="AS51" s="88" t="s">
+        <v>285</v>
+      </c>
+      <c r="AT51" s="88" t="s">
+        <v>298</v>
+      </c>
+      <c r="AU51" s="88" t="s">
+        <v>313</v>
+      </c>
+      <c r="AV51" s="88" t="s">
+        <v>306</v>
+      </c>
+      <c r="AW51" s="88" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="52" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A52" s="32"/>
       <c r="B52" s="28"/>
       <c r="C52" s="28"/>
       <c r="D52" s="28"/>
       <c r="E52" s="28"/>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A53" s="32"/>
       <c r="B53" s="6"/>
       <c r="C53" s="6"/>
@@ -3344,8 +3797,9 @@
       <c r="G53" s="6"/>
       <c r="H53" s="6"/>
       <c r="I53" s="6"/>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="AS53" s="1"/>
+    </row>
+    <row r="54" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A54" s="6"/>
       <c r="B54" s="30"/>
       <c r="C54" s="6"/>
@@ -3355,8 +3809,17 @@
       <c r="G54" s="6"/>
       <c r="H54" s="6"/>
       <c r="I54" s="6"/>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="AO54" s="89" t="s">
+        <v>314</v>
+      </c>
+      <c r="AR54" s="62"/>
+      <c r="AS54" s="62"/>
+      <c r="AT54" s="62"/>
+      <c r="AU54" s="62"/>
+      <c r="AV54" s="62"/>
+      <c r="AW54" s="62"/>
+    </row>
+    <row r="55" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A55" s="6"/>
       <c r="B55" s="6"/>
       <c r="C55" s="6"/>
@@ -3366,8 +3829,20 @@
       <c r="G55" s="6"/>
       <c r="H55" s="6"/>
       <c r="I55" s="6"/>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="AO55" t="s">
+        <v>114</v>
+      </c>
+      <c r="AP55" s="14">
+        <v>152</v>
+      </c>
+      <c r="AR55" s="62"/>
+      <c r="AS55" s="62"/>
+      <c r="AT55" s="62"/>
+      <c r="AU55" s="62"/>
+      <c r="AV55" s="62"/>
+      <c r="AW55" s="62"/>
+    </row>
+    <row r="56" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A56" s="6"/>
       <c r="B56" s="6"/>
       <c r="C56" s="6"/>
@@ -3377,8 +3852,14 @@
       <c r="G56" s="6"/>
       <c r="H56" s="6"/>
       <c r="I56" s="6"/>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="AO56" t="s">
+        <v>115</v>
+      </c>
+      <c r="AP56" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="57" spans="1:50" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="28"/>
       <c r="B57" s="27"/>
       <c r="C57" s="27"/>
@@ -3388,8 +3869,17 @@
       <c r="G57" s="27"/>
       <c r="H57" s="27"/>
       <c r="I57" s="27"/>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="AO57" t="s">
+        <v>103</v>
+      </c>
+      <c r="AP57" t="s">
+        <v>117</v>
+      </c>
+      <c r="AQ57" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="58" spans="1:50" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="6"/>
       <c r="B58" s="29"/>
       <c r="C58" s="29"/>
@@ -3399,8 +3889,35 @@
       <c r="G58" s="29"/>
       <c r="H58" s="29"/>
       <c r="I58" s="29"/>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="AO58" s="63" t="s">
+        <v>94</v>
+      </c>
+      <c r="AP58" s="64" t="s">
+        <v>95</v>
+      </c>
+      <c r="AQ58" s="64" t="s">
+        <v>96</v>
+      </c>
+      <c r="AR58" s="64" t="s">
+        <v>103</v>
+      </c>
+      <c r="AS58" s="64" t="s">
+        <v>102</v>
+      </c>
+      <c r="AT58" s="64" t="s">
+        <v>104</v>
+      </c>
+      <c r="AU58" s="64" t="s">
+        <v>101</v>
+      </c>
+      <c r="AV58" s="64" t="s">
+        <v>43</v>
+      </c>
+      <c r="AW58" s="65" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="59" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A59" s="6"/>
       <c r="B59" s="29"/>
       <c r="C59" s="29"/>
@@ -3410,8 +3927,35 @@
       <c r="G59" s="29"/>
       <c r="H59" s="29"/>
       <c r="I59" s="29"/>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="AO59" s="90" t="s">
+        <v>152</v>
+      </c>
+      <c r="AP59" s="91">
+        <v>24</v>
+      </c>
+      <c r="AQ59" s="91">
+        <v>30</v>
+      </c>
+      <c r="AR59" s="91" t="s">
+        <v>59</v>
+      </c>
+      <c r="AS59" s="91" t="s">
+        <v>285</v>
+      </c>
+      <c r="AT59" s="91" t="s">
+        <v>254</v>
+      </c>
+      <c r="AU59" s="91" t="s">
+        <v>256</v>
+      </c>
+      <c r="AV59" s="91" t="s">
+        <v>329</v>
+      </c>
+      <c r="AW59" s="92" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="60" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A60" s="6"/>
       <c r="B60" s="29"/>
       <c r="C60" s="29"/>
@@ -3421,8 +3965,35 @@
       <c r="G60" s="29"/>
       <c r="H60" s="29"/>
       <c r="I60" s="29"/>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="AO60" s="93" t="s">
+        <v>154</v>
+      </c>
+      <c r="AP60" s="94">
+        <v>24</v>
+      </c>
+      <c r="AQ60" s="94">
+        <v>30</v>
+      </c>
+      <c r="AR60" s="94" t="s">
+        <v>59</v>
+      </c>
+      <c r="AS60" s="94" t="s">
+        <v>285</v>
+      </c>
+      <c r="AT60" s="94" t="s">
+        <v>317</v>
+      </c>
+      <c r="AU60" s="94" t="s">
+        <v>336</v>
+      </c>
+      <c r="AV60" s="94" t="s">
+        <v>330</v>
+      </c>
+      <c r="AW60" s="95" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="61" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A61" s="6"/>
       <c r="B61" s="29"/>
       <c r="C61" s="29"/>
@@ -3432,22 +4003,107 @@
       <c r="G61" s="29"/>
       <c r="H61" s="29"/>
       <c r="I61" s="29"/>
-    </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="AO61" s="93" t="s">
+        <v>289</v>
+      </c>
+      <c r="AP61" s="94">
+        <v>23</v>
+      </c>
+      <c r="AQ61" s="94">
+        <v>30</v>
+      </c>
+      <c r="AR61" s="94" t="s">
+        <v>59</v>
+      </c>
+      <c r="AS61" s="94" t="s">
+        <v>285</v>
+      </c>
+      <c r="AT61" s="94" t="s">
+        <v>319</v>
+      </c>
+      <c r="AU61" s="94" t="s">
+        <v>337</v>
+      </c>
+      <c r="AV61" s="94" t="s">
+        <v>331</v>
+      </c>
+      <c r="AW61" s="95" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="62" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A62" s="6"/>
       <c r="B62" s="6"/>
       <c r="C62" s="6"/>
       <c r="D62" s="6"/>
       <c r="E62" s="6"/>
-    </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="AN62" s="6"/>
+      <c r="AO62" s="93" t="s">
+        <v>151</v>
+      </c>
+      <c r="AP62" s="94">
+        <v>21</v>
+      </c>
+      <c r="AQ62" s="94">
+        <v>30</v>
+      </c>
+      <c r="AR62" s="94" t="s">
+        <v>59</v>
+      </c>
+      <c r="AS62" s="94" t="s">
+        <v>285</v>
+      </c>
+      <c r="AT62" s="94" t="s">
+        <v>321</v>
+      </c>
+      <c r="AU62" s="94" t="s">
+        <v>338</v>
+      </c>
+      <c r="AV62" s="94" t="s">
+        <v>332</v>
+      </c>
+      <c r="AW62" s="95" t="s">
+        <v>322</v>
+      </c>
+      <c r="AX62" s="62"/>
+    </row>
+    <row r="63" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A63" s="6"/>
       <c r="B63" s="6"/>
       <c r="C63" s="6"/>
       <c r="D63" s="6"/>
       <c r="E63" s="6"/>
-    </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="AN63" s="6"/>
+      <c r="AO63" s="93" t="s">
+        <v>153</v>
+      </c>
+      <c r="AP63" s="94">
+        <v>20</v>
+      </c>
+      <c r="AQ63" s="94">
+        <v>30</v>
+      </c>
+      <c r="AR63" s="94" t="s">
+        <v>59</v>
+      </c>
+      <c r="AS63" s="94" t="s">
+        <v>285</v>
+      </c>
+      <c r="AT63" s="94" t="s">
+        <v>323</v>
+      </c>
+      <c r="AU63" s="94" t="s">
+        <v>339</v>
+      </c>
+      <c r="AV63" s="94" t="s">
+        <v>333</v>
+      </c>
+      <c r="AW63" s="95" t="s">
+        <v>324</v>
+      </c>
+      <c r="AX63" s="62"/>
+    </row>
+    <row r="64" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A64" s="32"/>
       <c r="B64" s="6"/>
       <c r="C64" s="6"/>
@@ -3457,8 +4113,37 @@
       <c r="G64" s="6"/>
       <c r="H64" s="6"/>
       <c r="I64" s="6"/>
-    </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="AN64" s="6"/>
+      <c r="AO64" s="93" t="s">
+        <v>150</v>
+      </c>
+      <c r="AP64" s="94">
+        <v>20</v>
+      </c>
+      <c r="AQ64" s="94">
+        <v>30</v>
+      </c>
+      <c r="AR64" s="94" t="s">
+        <v>59</v>
+      </c>
+      <c r="AS64" s="94" t="s">
+        <v>285</v>
+      </c>
+      <c r="AT64" s="94" t="s">
+        <v>325</v>
+      </c>
+      <c r="AU64" s="94" t="s">
+        <v>340</v>
+      </c>
+      <c r="AV64" s="94" t="s">
+        <v>334</v>
+      </c>
+      <c r="AW64" s="95" t="s">
+        <v>326</v>
+      </c>
+      <c r="AX64" s="62"/>
+    </row>
+    <row r="65" spans="1:50" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A65" s="6"/>
       <c r="B65" s="30"/>
       <c r="C65" s="6"/>
@@ -3468,8 +4153,37 @@
       <c r="G65" s="6"/>
       <c r="H65" s="6"/>
       <c r="I65" s="6"/>
-    </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="AN65" s="6"/>
+      <c r="AO65" s="96" t="s">
+        <v>149</v>
+      </c>
+      <c r="AP65" s="97">
+        <v>20</v>
+      </c>
+      <c r="AQ65" s="97">
+        <v>30</v>
+      </c>
+      <c r="AR65" s="97" t="s">
+        <v>59</v>
+      </c>
+      <c r="AS65" s="97" t="s">
+        <v>285</v>
+      </c>
+      <c r="AT65" s="97" t="s">
+        <v>327</v>
+      </c>
+      <c r="AU65" s="97" t="s">
+        <v>341</v>
+      </c>
+      <c r="AV65" s="97" t="s">
+        <v>335</v>
+      </c>
+      <c r="AW65" s="98" t="s">
+        <v>328</v>
+      </c>
+      <c r="AX65" s="62"/>
+    </row>
+    <row r="66" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A66" s="6"/>
       <c r="B66" s="6"/>
       <c r="C66" s="6"/>
@@ -3479,8 +4193,19 @@
       <c r="G66" s="6"/>
       <c r="H66" s="6"/>
       <c r="I66" s="6"/>
-    </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="AN66" s="6"/>
+      <c r="AO66" s="6"/>
+      <c r="AP66" s="6"/>
+      <c r="AQ66" s="6"/>
+      <c r="AR66" s="6"/>
+      <c r="AS66" s="6"/>
+      <c r="AT66" s="6"/>
+      <c r="AU66" s="6"/>
+      <c r="AV66" s="6"/>
+      <c r="AW66" s="6"/>
+      <c r="AX66" s="62"/>
+    </row>
+    <row r="67" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A67" s="6"/>
       <c r="B67" s="6"/>
       <c r="C67" s="6"/>
@@ -3490,8 +4215,17 @@
       <c r="G67" s="6"/>
       <c r="H67" s="6"/>
       <c r="I67" s="6"/>
-    </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="AN67" s="2"/>
+      <c r="AO67" s="2"/>
+      <c r="AP67" s="2"/>
+      <c r="AQ67" s="2"/>
+      <c r="AS67" s="2"/>
+      <c r="AT67" s="2"/>
+      <c r="AU67" s="2"/>
+      <c r="AV67" s="2"/>
+      <c r="AW67" s="2"/>
+    </row>
+    <row r="68" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A68" s="28"/>
       <c r="B68" s="27"/>
       <c r="C68" s="27"/>
@@ -3502,7 +4236,7 @@
       <c r="H68" s="27"/>
       <c r="I68" s="27"/>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A69" s="6"/>
       <c r="B69" s="29"/>
       <c r="C69" s="29"/>
@@ -3512,8 +4246,17 @@
       <c r="G69" s="29"/>
       <c r="H69" s="29"/>
       <c r="I69" s="29"/>
-    </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="AO69" s="89" t="s">
+        <v>342</v>
+      </c>
+      <c r="AR69" s="62"/>
+      <c r="AS69" s="62"/>
+      <c r="AT69" s="62"/>
+      <c r="AU69" s="62"/>
+      <c r="AV69" s="62"/>
+      <c r="AW69" s="62"/>
+    </row>
+    <row r="70" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A70" s="6"/>
       <c r="B70" s="29"/>
       <c r="C70" s="29"/>
@@ -3523,8 +4266,20 @@
       <c r="G70" s="29"/>
       <c r="H70" s="29"/>
       <c r="I70" s="29"/>
-    </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="AO70" t="s">
+        <v>114</v>
+      </c>
+      <c r="AP70" s="14">
+        <v>146</v>
+      </c>
+      <c r="AR70" s="62"/>
+      <c r="AS70" s="62"/>
+      <c r="AT70" s="62"/>
+      <c r="AU70" s="62"/>
+      <c r="AV70" s="62"/>
+      <c r="AW70" s="62"/>
+    </row>
+    <row r="71" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A71" s="6"/>
       <c r="B71" s="29"/>
       <c r="C71" s="29"/>
@@ -3534,8 +4289,14 @@
       <c r="G71" s="29"/>
       <c r="H71" s="29"/>
       <c r="I71" s="29"/>
-    </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="AO71" t="s">
+        <v>115</v>
+      </c>
+      <c r="AP71" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="72" spans="1:50" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A72" s="6"/>
       <c r="B72" s="29"/>
       <c r="C72" s="29"/>
@@ -3545,169 +4306,646 @@
       <c r="G72" s="29"/>
       <c r="H72" s="29"/>
       <c r="I72" s="29"/>
-    </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="AO72" t="s">
+        <v>103</v>
+      </c>
+      <c r="AP72" t="s">
+        <v>117</v>
+      </c>
+      <c r="AQ72" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="73" spans="1:50" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A73" s="6"/>
       <c r="B73" s="6"/>
       <c r="C73" s="6"/>
       <c r="D73" s="6"/>
       <c r="E73" s="6"/>
-    </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="AO73" s="63" t="s">
+        <v>94</v>
+      </c>
+      <c r="AP73" s="64" t="s">
+        <v>95</v>
+      </c>
+      <c r="AQ73" s="64" t="s">
+        <v>96</v>
+      </c>
+      <c r="AR73" s="64" t="s">
+        <v>103</v>
+      </c>
+      <c r="AS73" s="64" t="s">
+        <v>102</v>
+      </c>
+      <c r="AT73" s="64" t="s">
+        <v>104</v>
+      </c>
+      <c r="AU73" s="64" t="s">
+        <v>101</v>
+      </c>
+      <c r="AV73" s="64" t="s">
+        <v>43</v>
+      </c>
+      <c r="AW73" s="65" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="74" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A74" s="6"/>
       <c r="B74" s="6"/>
       <c r="C74" s="6"/>
       <c r="D74" s="6"/>
       <c r="E74" s="6"/>
-    </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="AO74" s="90" t="s">
+        <v>151</v>
+      </c>
+      <c r="AP74" s="91">
+        <v>24</v>
+      </c>
+      <c r="AQ74" s="91">
+        <v>30</v>
+      </c>
+      <c r="AR74" s="91" t="s">
+        <v>59</v>
+      </c>
+      <c r="AS74" s="91" t="s">
+        <v>285</v>
+      </c>
+      <c r="AT74" s="91" t="s">
+        <v>255</v>
+      </c>
+      <c r="AU74" s="91" t="s">
+        <v>257</v>
+      </c>
+      <c r="AV74" s="91" t="s">
+        <v>356</v>
+      </c>
+      <c r="AW74" s="92" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="75" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A75" s="6"/>
       <c r="B75" s="6"/>
       <c r="C75" s="6"/>
       <c r="D75" s="6"/>
       <c r="E75" s="6"/>
-    </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="AO75" s="93" t="s">
+        <v>289</v>
+      </c>
+      <c r="AP75" s="94">
+        <v>23</v>
+      </c>
+      <c r="AQ75" s="94">
+        <v>30</v>
+      </c>
+      <c r="AR75" s="94" t="s">
+        <v>59</v>
+      </c>
+      <c r="AS75" s="94" t="s">
+        <v>285</v>
+      </c>
+      <c r="AT75" s="94" t="s">
+        <v>344</v>
+      </c>
+      <c r="AU75" s="94" t="s">
+        <v>363</v>
+      </c>
+      <c r="AV75" s="94" t="s">
+        <v>357</v>
+      </c>
+      <c r="AW75" s="95" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="76" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A76" s="6"/>
       <c r="B76" s="6"/>
       <c r="C76" s="6"/>
       <c r="D76" s="6"/>
       <c r="E76" s="6"/>
-    </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="AO76" s="93" t="s">
+        <v>150</v>
+      </c>
+      <c r="AP76" s="94">
+        <v>22</v>
+      </c>
+      <c r="AQ76" s="94">
+        <v>30</v>
+      </c>
+      <c r="AR76" s="94" t="s">
+        <v>59</v>
+      </c>
+      <c r="AS76" s="94" t="s">
+        <v>285</v>
+      </c>
+      <c r="AT76" s="94" t="s">
+        <v>346</v>
+      </c>
+      <c r="AU76" s="94" t="s">
+        <v>364</v>
+      </c>
+      <c r="AV76" s="94" t="s">
+        <v>358</v>
+      </c>
+      <c r="AW76" s="95" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="77" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A77" s="6"/>
       <c r="B77" s="6"/>
       <c r="C77" s="6"/>
       <c r="D77" s="6"/>
       <c r="E77" s="6"/>
-    </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="AO77" s="93" t="s">
+        <v>153</v>
+      </c>
+      <c r="AP77" s="94">
+        <v>20</v>
+      </c>
+      <c r="AQ77" s="94">
+        <v>30</v>
+      </c>
+      <c r="AR77" s="94" t="s">
+        <v>59</v>
+      </c>
+      <c r="AS77" s="94" t="s">
+        <v>285</v>
+      </c>
+      <c r="AT77" s="94" t="s">
+        <v>348</v>
+      </c>
+      <c r="AU77" s="94" t="s">
+        <v>365</v>
+      </c>
+      <c r="AV77" s="94" t="s">
+        <v>359</v>
+      </c>
+      <c r="AW77" s="95" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="78" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A78" s="6"/>
       <c r="B78" s="6"/>
       <c r="C78" s="6"/>
       <c r="D78" s="6"/>
       <c r="E78" s="6"/>
-    </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="AO78" s="93" t="s">
+        <v>149</v>
+      </c>
+      <c r="AP78" s="94">
+        <v>20</v>
+      </c>
+      <c r="AQ78" s="94">
+        <v>30</v>
+      </c>
+      <c r="AR78" s="94" t="s">
+        <v>59</v>
+      </c>
+      <c r="AS78" s="94" t="s">
+        <v>285</v>
+      </c>
+      <c r="AT78" s="94" t="s">
+        <v>350</v>
+      </c>
+      <c r="AU78" s="94" t="s">
+        <v>366</v>
+      </c>
+      <c r="AV78" s="94" t="s">
+        <v>360</v>
+      </c>
+      <c r="AW78" s="95" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="79" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A79" s="6"/>
       <c r="B79" s="6"/>
       <c r="C79" s="6"/>
       <c r="D79" s="6"/>
       <c r="E79" s="6"/>
-    </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="AO79" s="93" t="s">
+        <v>154</v>
+      </c>
+      <c r="AP79" s="94">
+        <v>19</v>
+      </c>
+      <c r="AQ79" s="94">
+        <v>30</v>
+      </c>
+      <c r="AR79" s="94" t="s">
+        <v>59</v>
+      </c>
+      <c r="AS79" s="94" t="s">
+        <v>285</v>
+      </c>
+      <c r="AT79" s="94" t="s">
+        <v>352</v>
+      </c>
+      <c r="AU79" s="94" t="s">
+        <v>367</v>
+      </c>
+      <c r="AV79" s="94" t="s">
+        <v>361</v>
+      </c>
+      <c r="AW79" s="95" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="80" spans="1:50" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A80" s="6"/>
       <c r="B80" s="6"/>
       <c r="C80" s="6"/>
       <c r="D80" s="6"/>
       <c r="E80" s="6"/>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="AO80" s="96" t="s">
+        <v>152</v>
+      </c>
+      <c r="AP80" s="97">
+        <v>18</v>
+      </c>
+      <c r="AQ80" s="97">
+        <v>30</v>
+      </c>
+      <c r="AR80" s="97" t="s">
+        <v>59</v>
+      </c>
+      <c r="AS80" s="97" t="s">
+        <v>285</v>
+      </c>
+      <c r="AT80" s="97" t="s">
+        <v>354</v>
+      </c>
+      <c r="AU80" s="97" t="s">
+        <v>368</v>
+      </c>
+      <c r="AV80" s="97" t="s">
+        <v>362</v>
+      </c>
+      <c r="AW80" s="98" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="81" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A81" s="6"/>
       <c r="B81" s="6"/>
       <c r="C81" s="6"/>
       <c r="D81" s="6"/>
       <c r="E81" s="6"/>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A82" s="6"/>
       <c r="B82" s="6"/>
       <c r="C82" s="6"/>
       <c r="D82" s="6"/>
       <c r="E82" s="6"/>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A83" s="6"/>
       <c r="B83" s="6"/>
       <c r="C83" s="6"/>
       <c r="D83" s="6"/>
       <c r="E83" s="6"/>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="AO83" s="89" t="s">
+        <v>369</v>
+      </c>
+      <c r="AR83" s="62"/>
+      <c r="AS83" s="62"/>
+      <c r="AT83" s="62"/>
+      <c r="AU83" s="62"/>
+      <c r="AV83" s="62"/>
+      <c r="AW83" s="62"/>
+    </row>
+    <row r="84" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A84" s="6"/>
       <c r="B84" s="6"/>
       <c r="C84" s="6"/>
       <c r="D84" s="6"/>
       <c r="E84" s="6"/>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="AO84" t="s">
+        <v>114</v>
+      </c>
+      <c r="AP84" s="14">
+        <v>138</v>
+      </c>
+      <c r="AR84" s="62"/>
+      <c r="AS84" s="62"/>
+      <c r="AT84" s="62"/>
+      <c r="AU84" s="62"/>
+      <c r="AV84" s="62"/>
+      <c r="AW84" s="62"/>
+    </row>
+    <row r="85" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A85" s="6"/>
       <c r="B85" s="6"/>
       <c r="C85" s="6"/>
       <c r="D85" s="6"/>
       <c r="E85" s="6"/>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="AO85" t="s">
+        <v>115</v>
+      </c>
+      <c r="AP85" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="86" spans="1:49" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A86" s="6"/>
       <c r="B86" s="6"/>
       <c r="C86" s="6"/>
       <c r="D86" s="6"/>
       <c r="E86" s="6"/>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="AO86" t="s">
+        <v>103</v>
+      </c>
+      <c r="AP86" t="s">
+        <v>117</v>
+      </c>
+      <c r="AQ86" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="87" spans="1:49" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A87" s="6"/>
       <c r="B87" s="6"/>
       <c r="C87" s="6"/>
       <c r="D87" s="6"/>
       <c r="E87" s="6"/>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="AO87" s="63" t="s">
+        <v>94</v>
+      </c>
+      <c r="AP87" s="64" t="s">
+        <v>95</v>
+      </c>
+      <c r="AQ87" s="64" t="s">
+        <v>96</v>
+      </c>
+      <c r="AR87" s="64" t="s">
+        <v>103</v>
+      </c>
+      <c r="AS87" s="64" t="s">
+        <v>102</v>
+      </c>
+      <c r="AT87" s="64" t="s">
+        <v>104</v>
+      </c>
+      <c r="AU87" s="64" t="s">
+        <v>101</v>
+      </c>
+      <c r="AV87" s="64" t="s">
+        <v>43</v>
+      </c>
+      <c r="AW87" s="65" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="88" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A88" s="6"/>
       <c r="B88" s="6"/>
       <c r="C88" s="6"/>
       <c r="D88" s="6"/>
       <c r="E88" s="6"/>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="AO88" s="90" t="s">
+        <v>153</v>
+      </c>
+      <c r="AP88" s="91">
+        <v>24</v>
+      </c>
+      <c r="AQ88" s="91">
+        <v>30</v>
+      </c>
+      <c r="AR88" s="91" t="s">
+        <v>315</v>
+      </c>
+      <c r="AS88" s="91" t="s">
+        <v>285</v>
+      </c>
+      <c r="AT88" s="91" t="s">
+        <v>59</v>
+      </c>
+      <c r="AU88" s="91" t="s">
+        <v>268</v>
+      </c>
+      <c r="AV88" s="91" t="s">
+        <v>385</v>
+      </c>
+      <c r="AW88" s="92" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="89" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A89" s="6"/>
       <c r="B89" s="6"/>
       <c r="C89" s="6"/>
       <c r="D89" s="6"/>
       <c r="E89" s="6"/>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="AO89" s="93" t="s">
+        <v>154</v>
+      </c>
+      <c r="AP89" s="94">
+        <v>23</v>
+      </c>
+      <c r="AQ89" s="94">
+        <v>30</v>
+      </c>
+      <c r="AR89" s="94" t="s">
+        <v>371</v>
+      </c>
+      <c r="AS89" s="94" t="s">
+        <v>285</v>
+      </c>
+      <c r="AT89" s="94" t="s">
+        <v>59</v>
+      </c>
+      <c r="AU89" s="94" t="s">
+        <v>390</v>
+      </c>
+      <c r="AV89" s="94" t="s">
+        <v>389</v>
+      </c>
+      <c r="AW89" s="95" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="90" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A90" s="6"/>
       <c r="B90" s="6"/>
       <c r="C90" s="6"/>
       <c r="D90" s="6"/>
       <c r="E90" s="6"/>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="AO90" s="93" t="s">
+        <v>149</v>
+      </c>
+      <c r="AP90" s="94">
+        <v>23</v>
+      </c>
+      <c r="AQ90" s="94">
+        <v>30</v>
+      </c>
+      <c r="AR90" s="94" t="s">
+        <v>373</v>
+      </c>
+      <c r="AS90" s="94" t="s">
+        <v>285</v>
+      </c>
+      <c r="AT90" s="94" t="s">
+        <v>59</v>
+      </c>
+      <c r="AU90" s="94" t="s">
+        <v>391</v>
+      </c>
+      <c r="AV90" s="94" t="s">
+        <v>372</v>
+      </c>
+      <c r="AW90" s="95" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="91" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A91" s="6"/>
       <c r="B91" s="6"/>
       <c r="C91" s="6"/>
       <c r="D91" s="6"/>
       <c r="E91" s="6"/>
-    </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="AO91" s="93" t="s">
+        <v>151</v>
+      </c>
+      <c r="AP91" s="94">
+        <v>20</v>
+      </c>
+      <c r="AQ91" s="94">
+        <v>30</v>
+      </c>
+      <c r="AR91" s="94" t="s">
+        <v>375</v>
+      </c>
+      <c r="AS91" s="94" t="s">
+        <v>285</v>
+      </c>
+      <c r="AT91" s="94" t="s">
+        <v>59</v>
+      </c>
+      <c r="AU91" s="94" t="s">
+        <v>392</v>
+      </c>
+      <c r="AV91" s="94" t="s">
+        <v>373</v>
+      </c>
+      <c r="AW91" s="95" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="92" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A92" s="6"/>
       <c r="B92" s="6"/>
       <c r="C92" s="6"/>
       <c r="D92" s="6"/>
       <c r="E92" s="6"/>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="AO92" s="93" t="s">
+        <v>289</v>
+      </c>
+      <c r="AP92" s="94">
+        <v>18</v>
+      </c>
+      <c r="AQ92" s="94">
+        <v>30</v>
+      </c>
+      <c r="AR92" s="94" t="s">
+        <v>377</v>
+      </c>
+      <c r="AS92" s="94" t="s">
+        <v>285</v>
+      </c>
+      <c r="AT92" s="94" t="s">
+        <v>59</v>
+      </c>
+      <c r="AU92" s="94" t="s">
+        <v>393</v>
+      </c>
+      <c r="AV92" s="94" t="s">
+        <v>386</v>
+      </c>
+      <c r="AW92" s="95" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="93" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A93" s="6"/>
       <c r="B93" s="6"/>
       <c r="C93" s="6"/>
       <c r="D93" s="6"/>
       <c r="E93" s="6"/>
-    </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="AO93" s="93" t="s">
+        <v>150</v>
+      </c>
+      <c r="AP93" s="94">
+        <v>17</v>
+      </c>
+      <c r="AQ93" s="94">
+        <v>30</v>
+      </c>
+      <c r="AR93" s="94" t="s">
+        <v>379</v>
+      </c>
+      <c r="AS93" s="94" t="s">
+        <v>285</v>
+      </c>
+      <c r="AT93" s="94" t="s">
+        <v>59</v>
+      </c>
+      <c r="AU93" s="94" t="s">
+        <v>394</v>
+      </c>
+      <c r="AV93" s="94" t="s">
+        <v>387</v>
+      </c>
+      <c r="AW93" s="95" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="94" spans="1:49" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A94" s="6"/>
       <c r="B94" s="6"/>
       <c r="C94" s="6"/>
       <c r="D94" s="6"/>
       <c r="E94" s="6"/>
-    </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="AO94" s="96" t="s">
+        <v>152</v>
+      </c>
+      <c r="AP94" s="97">
+        <v>13</v>
+      </c>
+      <c r="AQ94" s="97">
+        <v>14</v>
+      </c>
+      <c r="AR94" s="97" t="s">
+        <v>381</v>
+      </c>
+      <c r="AS94" s="97" t="s">
+        <v>382</v>
+      </c>
+      <c r="AT94" s="97" t="s">
+        <v>383</v>
+      </c>
+      <c r="AU94" s="97" t="s">
+        <v>395</v>
+      </c>
+      <c r="AV94" s="94" t="s">
+        <v>388</v>
+      </c>
+      <c r="AW94" s="98" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="95" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A95" s="6"/>
       <c r="B95" s="6"/>
       <c r="C95" s="6"/>
       <c r="D95" s="6"/>
       <c r="E95" s="6"/>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A96" s="6"/>
       <c r="B96" s="6"/>
       <c r="C96" s="6"/>
@@ -3815,160 +5053,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C11:J15"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J12" sqref="J12:J15"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="3" max="3" width="18.28515625" customWidth="1"/>
-    <col min="4" max="4" width="21" customWidth="1"/>
-    <col min="8" max="8" width="17.42578125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="11" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C11" t="s">
-        <v>94</v>
-      </c>
-      <c r="D11" t="s">
-        <v>95</v>
-      </c>
-      <c r="E11" t="s">
-        <v>96</v>
-      </c>
-      <c r="F11" t="s">
-        <v>217</v>
-      </c>
-      <c r="G11" t="s">
-        <v>218</v>
-      </c>
-      <c r="H11" t="s">
-        <v>219</v>
-      </c>
-      <c r="I11" t="s">
-        <v>220</v>
-      </c>
-      <c r="J11" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="12" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C12">
-        <v>1</v>
-      </c>
-      <c r="D12">
-        <v>153</v>
-      </c>
-      <c r="E12">
-        <v>254</v>
-      </c>
-      <c r="F12" t="s">
-        <v>4</v>
-      </c>
-      <c r="G12" t="s">
-        <v>116</v>
-      </c>
-      <c r="H12" t="s">
-        <v>117</v>
-      </c>
-      <c r="I12" t="s">
-        <v>238</v>
-      </c>
-      <c r="J12" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="13" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C13">
-        <v>2</v>
-      </c>
-      <c r="D13">
-        <v>152</v>
-      </c>
-      <c r="E13">
-        <v>254</v>
-      </c>
-      <c r="F13" t="s">
-        <v>75</v>
-      </c>
-      <c r="G13" t="s">
-        <v>116</v>
-      </c>
-      <c r="H13" t="s">
-        <v>117</v>
-      </c>
-      <c r="I13" t="s">
-        <v>239</v>
-      </c>
-      <c r="J13" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="14" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C14">
-        <v>3</v>
-      </c>
-      <c r="D14">
-        <v>143</v>
-      </c>
-      <c r="E14">
-        <v>254</v>
-      </c>
-      <c r="F14" t="s">
-        <v>7</v>
-      </c>
-      <c r="G14" t="s">
-        <v>116</v>
-      </c>
-      <c r="H14" t="s">
-        <v>117</v>
-      </c>
-      <c r="I14" t="s">
-        <v>240</v>
-      </c>
-      <c r="J14" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="15" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C15" t="s">
-        <v>241</v>
-      </c>
-      <c r="D15">
-        <v>143</v>
-      </c>
-      <c r="E15">
-        <v>254</v>
-      </c>
-      <c r="F15" t="s">
-        <v>242</v>
-      </c>
-      <c r="G15" t="s">
-        <v>116</v>
-      </c>
-      <c r="H15" t="s">
-        <v>117</v>
-      </c>
-      <c r="I15" t="s">
-        <v>243</v>
-      </c>
-      <c r="J15" t="s">
-        <v>9</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3999,69 +5087,69 @@
     <row r="3" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="19"/>
-      <c r="B4" s="66" t="s">
+      <c r="B4" s="79" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="67"/>
-      <c r="D4" s="67"/>
-      <c r="E4" s="68"/>
-      <c r="F4" s="66" t="s">
+      <c r="C4" s="80"/>
+      <c r="D4" s="80"/>
+      <c r="E4" s="81"/>
+      <c r="F4" s="79" t="s">
         <v>24</v>
       </c>
-      <c r="G4" s="67"/>
-      <c r="H4" s="67"/>
-      <c r="I4" s="68"/>
-      <c r="J4" s="66" t="s">
+      <c r="G4" s="80"/>
+      <c r="H4" s="80"/>
+      <c r="I4" s="81"/>
+      <c r="J4" s="79" t="s">
         <v>26</v>
       </c>
-      <c r="K4" s="67"/>
-      <c r="L4" s="67"/>
-      <c r="M4" s="67"/>
-      <c r="N4" s="66" t="s">
+      <c r="K4" s="80"/>
+      <c r="L4" s="80"/>
+      <c r="M4" s="80"/>
+      <c r="N4" s="79" t="s">
         <v>27</v>
       </c>
-      <c r="O4" s="67"/>
-      <c r="P4" s="67"/>
-      <c r="Q4" s="68"/>
-      <c r="R4" s="66" t="s">
+      <c r="O4" s="80"/>
+      <c r="P4" s="80"/>
+      <c r="Q4" s="81"/>
+      <c r="R4" s="79" t="s">
         <v>25</v>
       </c>
-      <c r="S4" s="67"/>
-      <c r="T4" s="67"/>
-      <c r="U4" s="68"/>
+      <c r="S4" s="80"/>
+      <c r="T4" s="80"/>
+      <c r="U4" s="81"/>
     </row>
     <row r="5" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="20"/>
-      <c r="B5" s="63" t="s">
+      <c r="B5" s="82" t="s">
         <v>82</v>
       </c>
-      <c r="C5" s="64"/>
-      <c r="D5" s="64"/>
-      <c r="E5" s="65"/>
-      <c r="F5" s="63" t="s">
+      <c r="C5" s="83"/>
+      <c r="D5" s="83"/>
+      <c r="E5" s="84"/>
+      <c r="F5" s="82" t="s">
         <v>82</v>
       </c>
-      <c r="G5" s="64"/>
-      <c r="H5" s="64"/>
-      <c r="I5" s="65"/>
-      <c r="J5" s="63" t="s">
+      <c r="G5" s="83"/>
+      <c r="H5" s="83"/>
+      <c r="I5" s="84"/>
+      <c r="J5" s="82" t="s">
         <v>82</v>
       </c>
-      <c r="K5" s="64"/>
-      <c r="L5" s="64"/>
-      <c r="M5" s="64"/>
-      <c r="N5" s="63" t="s">
+      <c r="K5" s="83"/>
+      <c r="L5" s="83"/>
+      <c r="M5" s="83"/>
+      <c r="N5" s="82" t="s">
         <v>82</v>
       </c>
-      <c r="O5" s="64"/>
-      <c r="P5" s="64"/>
-      <c r="Q5" s="65"/>
-      <c r="R5" s="63" t="s">
+      <c r="O5" s="83"/>
+      <c r="P5" s="83"/>
+      <c r="Q5" s="84"/>
+      <c r="R5" s="82" t="s">
         <v>82</v>
       </c>
-      <c r="S5" s="64"/>
-      <c r="T5" s="64"/>
-      <c r="U5" s="65"/>
+      <c r="S5" s="83"/>
+      <c r="T5" s="83"/>
+      <c r="U5" s="84"/>
     </row>
     <row r="6" spans="1:21" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="22" t="s">
@@ -4674,69 +5762,69 @@
     </row>
     <row r="15" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="21"/>
-      <c r="B15" s="69">
+      <c r="B15" s="76">
         <f>B14+C14+D14+E14</f>
         <v>579</v>
       </c>
-      <c r="C15" s="70"/>
-      <c r="D15" s="70"/>
-      <c r="E15" s="71"/>
-      <c r="F15" s="69">
+      <c r="C15" s="77"/>
+      <c r="D15" s="77"/>
+      <c r="E15" s="78"/>
+      <c r="F15" s="76">
         <f>F14+G14+H14+I14</f>
         <v>585</v>
       </c>
-      <c r="G15" s="70"/>
-      <c r="H15" s="70"/>
-      <c r="I15" s="71"/>
-      <c r="J15" s="69">
+      <c r="G15" s="77"/>
+      <c r="H15" s="77"/>
+      <c r="I15" s="78"/>
+      <c r="J15" s="76">
         <f>J14+K14+L14+M14</f>
         <v>580</v>
       </c>
-      <c r="K15" s="70"/>
-      <c r="L15" s="70"/>
-      <c r="M15" s="70"/>
-      <c r="N15" s="69">
+      <c r="K15" s="77"/>
+      <c r="L15" s="77"/>
+      <c r="M15" s="77"/>
+      <c r="N15" s="76">
         <f>N14+O14+P14+Q14</f>
         <v>590</v>
       </c>
-      <c r="O15" s="70"/>
-      <c r="P15" s="70"/>
-      <c r="Q15" s="71"/>
-      <c r="R15" s="69">
+      <c r="O15" s="77"/>
+      <c r="P15" s="77"/>
+      <c r="Q15" s="78"/>
+      <c r="R15" s="76">
         <f>R14+S14+T14+U14</f>
         <v>571</v>
       </c>
-      <c r="S15" s="70"/>
-      <c r="T15" s="70"/>
-      <c r="U15" s="71"/>
+      <c r="S15" s="77"/>
+      <c r="T15" s="77"/>
+      <c r="U15" s="78"/>
     </row>
     <row r="20" spans="12:12" x14ac:dyDescent="0.25">
       <c r="L20" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="F5:I5"/>
+    <mergeCell ref="J5:M5"/>
+    <mergeCell ref="N5:Q5"/>
+    <mergeCell ref="R5:U5"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="F4:I4"/>
+    <mergeCell ref="J4:M4"/>
+    <mergeCell ref="N4:Q4"/>
+    <mergeCell ref="R4:U4"/>
     <mergeCell ref="B15:E15"/>
     <mergeCell ref="F15:I15"/>
     <mergeCell ref="J15:M15"/>
     <mergeCell ref="N15:Q15"/>
     <mergeCell ref="R15:U15"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="F4:I4"/>
-    <mergeCell ref="J4:M4"/>
-    <mergeCell ref="N4:Q4"/>
-    <mergeCell ref="R4:U4"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="F5:I5"/>
-    <mergeCell ref="J5:M5"/>
-    <mergeCell ref="N5:Q5"/>
-    <mergeCell ref="R5:U5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:L26"/>
   <sheetViews>
@@ -5182,7 +6270,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W126"/>
   <sheetViews>
@@ -5197,23 +6285,23 @@
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="19"/>
-      <c r="B1" s="66" t="s">
+      <c r="B1" s="79" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="67"/>
-      <c r="D1" s="67"/>
-      <c r="E1" s="68"/>
+      <c r="C1" s="80"/>
+      <c r="D1" s="80"/>
+      <c r="E1" s="81"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="24" t="s">
         <v>81</v>
       </c>
-      <c r="B2" s="63" t="s">
+      <c r="B2" s="82" t="s">
         <v>82</v>
       </c>
-      <c r="C2" s="64"/>
-      <c r="D2" s="64"/>
-      <c r="E2" s="65"/>
+      <c r="C2" s="83"/>
+      <c r="D2" s="83"/>
+      <c r="E2" s="84"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
@@ -5370,13 +6458,13 @@
     </row>
     <row r="12" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="21"/>
-      <c r="B12" s="69">
+      <c r="B12" s="76">
         <f>B11+C11+D11+E11</f>
         <v>322</v>
       </c>
-      <c r="C12" s="70"/>
-      <c r="D12" s="70"/>
-      <c r="E12" s="71"/>
+      <c r="C12" s="77"/>
+      <c r="D12" s="77"/>
+      <c r="E12" s="78"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">

</xml_diff>

<commit_message>
Agregar Configuracion dhcp y subneteo para red de cajas
</commit_message>
<xml_diff>
--- a/SUBNETEO REDES.xlsx
+++ b/SUBNETEO REDES.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1167" uniqueCount="396">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1204" uniqueCount="412">
   <si>
     <t>REDES:5</t>
   </si>
@@ -584,9 +584,6 @@
     <t>S3</t>
   </si>
   <si>
-    <t>50 maquinas</t>
-  </si>
-  <si>
     <t>156 computadoras</t>
   </si>
   <si>
@@ -599,30 +596,9 @@
     <t>Seccion 3</t>
   </si>
   <si>
-    <t>20</t>
-  </si>
-  <si>
-    <t>10</t>
-  </si>
-  <si>
-    <t>1-8</t>
-  </si>
-  <si>
     <t>1-4</t>
   </si>
   <si>
-    <t>9-16</t>
-  </si>
-  <si>
-    <t>17-20</t>
-  </si>
-  <si>
-    <t>17-19</t>
-  </si>
-  <si>
-    <t>9-12</t>
-  </si>
-  <si>
     <t>WALMART COSTA RICA</t>
   </si>
   <si>
@@ -1215,6 +1191,78 @@
   </si>
   <si>
     <t xml:space="preserve">172.168.28.193 </t>
+  </si>
+  <si>
+    <t>42 maquinas</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>1-5</t>
+  </si>
+  <si>
+    <t>6-10</t>
+  </si>
+  <si>
+    <t>6-9</t>
+  </si>
+  <si>
+    <t>11-15</t>
+  </si>
+  <si>
+    <t>11-14</t>
+  </si>
+  <si>
+    <t>Sub Red Cajas</t>
+  </si>
+  <si>
+    <t>255.255.254.192</t>
+  </si>
+  <si>
+    <t>SECCION 1</t>
+  </si>
+  <si>
+    <t>/ 28</t>
+  </si>
+  <si>
+    <t>172.168.25.15</t>
+  </si>
+  <si>
+    <t>SECCION 2</t>
+  </si>
+  <si>
+    <t>172.168.25.16</t>
+  </si>
+  <si>
+    <t>172.168.25.31</t>
+  </si>
+  <si>
+    <t>SECCION 3</t>
+  </si>
+  <si>
+    <t>172.168.25.32</t>
+  </si>
+  <si>
+    <t>172.168.25.47</t>
+  </si>
+  <si>
+    <t>172.168.25.14</t>
+  </si>
+  <si>
+    <t>172.168.25.30</t>
+  </si>
+  <si>
+    <t>172.168.25.46</t>
+  </si>
+  <si>
+    <t xml:space="preserve">172.168.25.1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">172.168.25.17 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">172.168.25.33 </t>
   </si>
 </sst>
 </file>
@@ -1246,7 +1294,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1310,6 +1358,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1495,7 +1555,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="99">
+  <cellXfs count="109">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -1638,33 +1698,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1695,6 +1728,55 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1985,8 +2067,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AX111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AI73" workbookViewId="0">
-      <selection activeCell="AU91" sqref="AU91"/>
+    <sheetView tabSelected="1" topLeftCell="AI47" workbookViewId="0">
+      <selection activeCell="AQ63" sqref="AQ63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2041,7 +2123,7 @@
         <v>0</v>
       </c>
       <c r="K1" t="s">
-        <v>213</v>
+        <v>205</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
@@ -2061,7 +2143,7 @@
         <v>0</v>
       </c>
       <c r="K2" t="s">
-        <v>214</v>
+        <v>206</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
@@ -2078,10 +2160,10 @@
         <v>0</v>
       </c>
       <c r="K3" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
       <c r="L3" t="s">
-        <v>216</v>
+        <v>208</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
@@ -2147,19 +2229,19 @@
         <v>96</v>
       </c>
       <c r="N6" t="s">
-        <v>217</v>
+        <v>209</v>
       </c>
       <c r="O6" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="P6" t="s">
-        <v>219</v>
+        <v>211</v>
       </c>
       <c r="Q6" t="s">
-        <v>220</v>
+        <v>212</v>
       </c>
       <c r="R6" t="s">
-        <v>221</v>
+        <v>213</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
@@ -2174,28 +2256,28 @@
         <v>91</v>
       </c>
       <c r="K7" t="s">
-        <v>222</v>
+        <v>214</v>
       </c>
       <c r="L7">
         <v>3</v>
       </c>
       <c r="M7" t="s">
-        <v>223</v>
+        <v>215</v>
       </c>
       <c r="N7" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
       <c r="O7" t="s">
-        <v>224</v>
+        <v>216</v>
       </c>
       <c r="P7" t="s">
-        <v>225</v>
+        <v>217</v>
       </c>
       <c r="Q7" t="s">
-        <v>226</v>
+        <v>218</v>
       </c>
       <c r="R7" t="s">
-        <v>227</v>
+        <v>219</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
@@ -2216,7 +2298,7 @@
     </row>
     <row r="11" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="28" t="s">
-        <v>228</v>
+        <v>220</v>
       </c>
     </row>
     <row r="12" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2260,10 +2342,10 @@
         <v>2046</v>
       </c>
       <c r="D13" s="37" t="s">
-        <v>229</v>
+        <v>221</v>
       </c>
       <c r="E13" s="37" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
       <c r="F13" s="37" t="s">
         <v>4</v>
@@ -2290,16 +2372,16 @@
         <v>2046</v>
       </c>
       <c r="D14" s="37" t="s">
-        <v>229</v>
+        <v>221</v>
       </c>
       <c r="E14" s="37" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
       <c r="F14" s="37" t="s">
         <v>12</v>
       </c>
       <c r="G14" s="37" t="s">
-        <v>234</v>
+        <v>226</v>
       </c>
       <c r="H14" s="37" t="s">
         <v>10</v>
@@ -2320,10 +2402,10 @@
         <v>2046</v>
       </c>
       <c r="D15" s="37" t="s">
-        <v>229</v>
+        <v>221</v>
       </c>
       <c r="E15" s="37" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
       <c r="F15" s="37" t="s">
         <v>93</v>
@@ -2350,16 +2432,16 @@
         <v>2046</v>
       </c>
       <c r="D16" s="37" t="s">
-        <v>229</v>
+        <v>221</v>
       </c>
       <c r="E16" s="37" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
       <c r="F16" s="37" t="s">
-        <v>232</v>
+        <v>224</v>
       </c>
       <c r="G16" s="37" t="s">
-        <v>235</v>
+        <v>227</v>
       </c>
       <c r="H16" s="37" t="s">
         <v>106</v>
@@ -2380,16 +2462,16 @@
         <v>2046</v>
       </c>
       <c r="D17" s="38" t="s">
-        <v>229</v>
+        <v>221</v>
       </c>
       <c r="E17" s="38" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
       <c r="F17" s="38" t="s">
-        <v>233</v>
+        <v>225</v>
       </c>
       <c r="G17" s="38" t="s">
-        <v>236</v>
+        <v>228</v>
       </c>
       <c r="H17" s="38" t="s">
         <v>107</v>
@@ -2462,7 +2544,7 @@
         <v>115</v>
       </c>
       <c r="B22" t="s">
-        <v>233</v>
+        <v>225</v>
       </c>
       <c r="K22" t="s">
         <v>115</v>
@@ -2494,19 +2576,19 @@
         <v>103</v>
       </c>
       <c r="B23" t="s">
-        <v>229</v>
+        <v>221</v>
       </c>
       <c r="C23" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
       <c r="K23" t="s">
         <v>103</v>
       </c>
       <c r="L23" t="s">
-        <v>229</v>
+        <v>221</v>
       </c>
       <c r="M23" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
       <c r="U23" t="s">
         <v>115</v>
@@ -2524,7 +2606,7 @@
         <v>115</v>
       </c>
       <c r="AP23" t="s">
-        <v>232</v>
+        <v>224</v>
       </c>
     </row>
     <row r="24" spans="1:49" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2587,25 +2669,25 @@
         <v>103</v>
       </c>
       <c r="V24" t="s">
-        <v>229</v>
+        <v>221</v>
       </c>
       <c r="W24" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
       <c r="AE24" t="s">
         <v>103</v>
       </c>
       <c r="AF24" t="s">
-        <v>237</v>
+        <v>229</v>
       </c>
       <c r="AO24" t="s">
         <v>103</v>
       </c>
       <c r="AP24" t="s">
-        <v>229</v>
+        <v>221</v>
       </c>
       <c r="AQ24" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
     </row>
     <row r="25" spans="1:49" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2625,16 +2707,16 @@
         <v>116</v>
       </c>
       <c r="F25" s="37" t="s">
-        <v>233</v>
+        <v>225</v>
       </c>
       <c r="G25" s="37" t="s">
-        <v>236</v>
+        <v>228</v>
       </c>
       <c r="H25" s="37" t="s">
-        <v>245</v>
+        <v>237</v>
       </c>
       <c r="I25" s="40" t="s">
-        <v>249</v>
+        <v>241</v>
       </c>
       <c r="J25" s="6"/>
       <c r="K25" s="33" t="s">
@@ -2763,16 +2845,16 @@
         <v>116</v>
       </c>
       <c r="F26" s="37" t="s">
-        <v>239</v>
+        <v>231</v>
       </c>
       <c r="G26" s="37" t="s">
+        <v>234</v>
+      </c>
+      <c r="H26" s="37" t="s">
+        <v>238</v>
+      </c>
+      <c r="I26" s="40" t="s">
         <v>242</v>
-      </c>
-      <c r="H26" s="37" t="s">
-        <v>246</v>
-      </c>
-      <c r="I26" s="40" t="s">
-        <v>250</v>
       </c>
       <c r="J26" s="6"/>
       <c r="K26" s="33" t="s">
@@ -2866,22 +2948,22 @@
         <v>254</v>
       </c>
       <c r="AR26" s="37" t="s">
-        <v>266</v>
+        <v>258</v>
       </c>
       <c r="AS26" s="37" t="s">
-        <v>231</v>
+        <v>223</v>
       </c>
       <c r="AT26" s="37" t="s">
-        <v>232</v>
+        <v>224</v>
       </c>
       <c r="AU26" s="37" t="s">
-        <v>235</v>
+        <v>227</v>
       </c>
       <c r="AV26" s="37" t="s">
-        <v>259</v>
+        <v>251</v>
       </c>
       <c r="AW26" s="37" t="s">
-        <v>263</v>
+        <v>255</v>
       </c>
     </row>
     <row r="27" spans="1:49" x14ac:dyDescent="0.25">
@@ -2901,16 +2983,16 @@
         <v>116</v>
       </c>
       <c r="F27" s="37" t="s">
-        <v>240</v>
+        <v>232</v>
       </c>
       <c r="G27" s="37" t="s">
-        <v>244</v>
+        <v>236</v>
       </c>
       <c r="H27" s="37" t="s">
-        <v>247</v>
+        <v>239</v>
       </c>
       <c r="I27" s="40" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="J27" s="6"/>
       <c r="K27" s="33" t="s">
@@ -2995,7 +3077,7 @@
         <v>120</v>
       </c>
       <c r="AO27" s="33" t="s">
-        <v>271</v>
+        <v>263</v>
       </c>
       <c r="AP27" s="37">
         <v>152</v>
@@ -3010,16 +3092,16 @@
         <v>116</v>
       </c>
       <c r="AT27" s="37" t="s">
-        <v>254</v>
+        <v>246</v>
       </c>
       <c r="AU27" s="37" t="s">
+        <v>248</v>
+      </c>
+      <c r="AV27" s="37" t="s">
+        <v>252</v>
+      </c>
+      <c r="AW27" s="37" t="s">
         <v>256</v>
-      </c>
-      <c r="AV27" s="37" t="s">
-        <v>260</v>
-      </c>
-      <c r="AW27" s="37" t="s">
-        <v>264</v>
       </c>
     </row>
     <row r="28" spans="1:49" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3039,16 +3121,16 @@
         <v>116</v>
       </c>
       <c r="F28" s="38" t="s">
-        <v>241</v>
+        <v>233</v>
       </c>
       <c r="G28" s="61" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="H28" s="38" t="s">
-        <v>248</v>
+        <v>240</v>
       </c>
       <c r="I28" s="41" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
       <c r="J28" s="6"/>
       <c r="K28" s="34" t="s">
@@ -3067,7 +3149,7 @@
         <v>116</v>
       </c>
       <c r="P28" s="38" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
       <c r="Q28" s="38" t="s">
         <v>144</v>
@@ -3148,16 +3230,16 @@
         <v>116</v>
       </c>
       <c r="AT28" s="37" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="AU28" s="37" t="s">
+        <v>249</v>
+      </c>
+      <c r="AV28" s="37" t="s">
+        <v>253</v>
+      </c>
+      <c r="AW28" s="37" t="s">
         <v>257</v>
-      </c>
-      <c r="AV28" s="37" t="s">
-        <v>261</v>
-      </c>
-      <c r="AW28" s="37" t="s">
-        <v>265</v>
       </c>
     </row>
     <row r="29" spans="1:49" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3236,16 +3318,16 @@
         <v>116</v>
       </c>
       <c r="AT29" s="38" t="s">
-        <v>315</v>
+        <v>307</v>
       </c>
       <c r="AU29" s="38" t="s">
-        <v>268</v>
+        <v>260</v>
       </c>
       <c r="AV29" s="38" t="s">
-        <v>269</v>
+        <v>261</v>
       </c>
       <c r="AW29" s="38" t="s">
-        <v>267</v>
+        <v>259</v>
       </c>
     </row>
     <row r="30" spans="1:49" x14ac:dyDescent="0.25">
@@ -3257,8 +3339,8 @@
     <row r="31" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A31" s="32"/>
       <c r="AN31" s="62"/>
-      <c r="AO31" s="89" t="s">
-        <v>270</v>
+      <c r="AO31" s="80" t="s">
+        <v>262</v>
       </c>
       <c r="AR31" s="62"/>
       <c r="AS31" s="62"/>
@@ -3289,7 +3371,7 @@
         <v>115</v>
       </c>
       <c r="AP33" t="s">
-        <v>232</v>
+        <v>224</v>
       </c>
     </row>
     <row r="34" spans="1:49" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3298,10 +3380,10 @@
         <v>103</v>
       </c>
       <c r="AP34" t="s">
-        <v>266</v>
+        <v>258</v>
       </c>
       <c r="AQ34" t="s">
-        <v>231</v>
+        <v>223</v>
       </c>
     </row>
     <row r="35" spans="1:49" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3355,7 +3437,7 @@
       <c r="I36" s="42"/>
       <c r="AN36" s="62"/>
       <c r="AO36" s="66" t="s">
-        <v>272</v>
+        <v>264</v>
       </c>
       <c r="AP36" s="67">
         <v>143</v>
@@ -3370,16 +3452,16 @@
         <v>116</v>
       </c>
       <c r="AT36" s="67" t="s">
-        <v>232</v>
+        <v>224</v>
       </c>
       <c r="AU36" s="67" t="s">
-        <v>235</v>
+        <v>227</v>
       </c>
       <c r="AV36" s="67" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
       <c r="AW36" s="68" t="s">
-        <v>262</v>
+        <v>254</v>
       </c>
     </row>
     <row r="37" spans="1:49" x14ac:dyDescent="0.25">
@@ -3393,7 +3475,7 @@
       <c r="H37" s="42"/>
       <c r="I37" s="42"/>
       <c r="AO37" s="66" t="s">
-        <v>273</v>
+        <v>265</v>
       </c>
       <c r="AP37" s="67">
         <v>50</v>
@@ -3402,22 +3484,22 @@
         <v>62</v>
       </c>
       <c r="AR37" s="67" t="s">
-        <v>275</v>
+        <v>267</v>
       </c>
       <c r="AS37" s="67" t="s">
+        <v>266</v>
+      </c>
+      <c r="AT37" s="67" t="s">
+        <v>245</v>
+      </c>
+      <c r="AU37" s="67" t="s">
         <v>274</v>
       </c>
-      <c r="AT37" s="67" t="s">
-        <v>253</v>
-      </c>
-      <c r="AU37" s="67" t="s">
-        <v>282</v>
-      </c>
       <c r="AV37" s="67" t="s">
-        <v>280</v>
+        <v>272</v>
       </c>
       <c r="AW37" s="68" t="s">
-        <v>276</v>
+        <v>268</v>
       </c>
     </row>
     <row r="38" spans="1:49" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3432,7 +3514,7 @@
       <c r="I38" s="42"/>
       <c r="AN38" s="75"/>
       <c r="AO38" s="69" t="s">
-        <v>277</v>
+        <v>269</v>
       </c>
       <c r="AP38" s="70">
         <v>50</v>
@@ -3441,22 +3523,22 @@
         <v>62</v>
       </c>
       <c r="AR38" s="70" t="s">
+        <v>267</v>
+      </c>
+      <c r="AS38" s="70" t="s">
+        <v>266</v>
+      </c>
+      <c r="AT38" s="70" t="s">
+        <v>270</v>
+      </c>
+      <c r="AU38" s="70" t="s">
         <v>275</v>
       </c>
-      <c r="AS38" s="70" t="s">
-        <v>274</v>
-      </c>
-      <c r="AT38" s="70" t="s">
-        <v>278</v>
-      </c>
-      <c r="AU38" s="70" t="s">
-        <v>283</v>
-      </c>
       <c r="AV38" s="70" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
       <c r="AW38" s="71" t="s">
-        <v>279</v>
+        <v>271</v>
       </c>
     </row>
     <row r="39" spans="1:49" x14ac:dyDescent="0.25">
@@ -3489,7 +3571,7 @@
       <c r="H40" s="42"/>
       <c r="I40" s="42"/>
       <c r="AO40" s="60" t="s">
-        <v>284</v>
+        <v>276</v>
       </c>
     </row>
     <row r="41" spans="1:49" x14ac:dyDescent="0.25">
@@ -3529,7 +3611,7 @@
         <v>115</v>
       </c>
       <c r="AP42" t="s">
-        <v>232</v>
+        <v>224</v>
       </c>
     </row>
     <row r="43" spans="1:49" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3573,177 +3655,177 @@
       </c>
     </row>
     <row r="45" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="AO45" s="85" t="s">
+      <c r="AO45" s="76" t="s">
         <v>151</v>
       </c>
-      <c r="AP45" s="86">
+      <c r="AP45" s="77">
         <v>23</v>
       </c>
-      <c r="AQ45" s="86">
+      <c r="AQ45" s="77">
         <v>30</v>
       </c>
-      <c r="AR45" s="86" t="s">
+      <c r="AR45" s="77" t="s">
         <v>59</v>
       </c>
-      <c r="AS45" s="86" t="s">
+      <c r="AS45" s="77" t="s">
+        <v>277</v>
+      </c>
+      <c r="AT45" s="77" t="s">
+        <v>224</v>
+      </c>
+      <c r="AU45" s="77" t="s">
+        <v>299</v>
+      </c>
+      <c r="AV45" s="77" t="s">
+        <v>292</v>
+      </c>
+      <c r="AW45" s="77" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="46" spans="1:49" x14ac:dyDescent="0.25">
+      <c r="AO46" s="76" t="s">
+        <v>150</v>
+      </c>
+      <c r="AP46" s="77">
+        <v>22</v>
+      </c>
+      <c r="AQ46" s="77">
+        <v>30</v>
+      </c>
+      <c r="AR46" s="77" t="s">
+        <v>59</v>
+      </c>
+      <c r="AS46" s="77" t="s">
+        <v>277</v>
+      </c>
+      <c r="AT46" s="77" t="s">
+        <v>279</v>
+      </c>
+      <c r="AU46" s="77" t="s">
+        <v>300</v>
+      </c>
+      <c r="AV46" s="77" t="s">
+        <v>293</v>
+      </c>
+      <c r="AW46" s="77" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="47" spans="1:49" x14ac:dyDescent="0.25">
+      <c r="AO47" s="76" t="s">
+        <v>281</v>
+      </c>
+      <c r="AP47" s="77">
+        <v>21</v>
+      </c>
+      <c r="AQ47" s="77">
+        <v>30</v>
+      </c>
+      <c r="AR47" s="77" t="s">
+        <v>59</v>
+      </c>
+      <c r="AS47" s="77" t="s">
+        <v>277</v>
+      </c>
+      <c r="AT47" s="77" t="s">
+        <v>282</v>
+      </c>
+      <c r="AU47" s="77" t="s">
+        <v>301</v>
+      </c>
+      <c r="AV47" s="77" t="s">
+        <v>294</v>
+      </c>
+      <c r="AW47" s="77" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="48" spans="1:49" x14ac:dyDescent="0.25">
+      <c r="AO48" s="76" t="s">
+        <v>153</v>
+      </c>
+      <c r="AP48" s="77">
+        <v>20</v>
+      </c>
+      <c r="AQ48" s="77">
+        <v>30</v>
+      </c>
+      <c r="AR48" s="77" t="s">
+        <v>59</v>
+      </c>
+      <c r="AS48" s="77" t="s">
+        <v>277</v>
+      </c>
+      <c r="AT48" s="77" t="s">
+        <v>284</v>
+      </c>
+      <c r="AU48" s="77" t="s">
+        <v>302</v>
+      </c>
+      <c r="AV48" s="77" t="s">
+        <v>295</v>
+      </c>
+      <c r="AW48" s="77" t="s">
         <v>285</v>
       </c>
-      <c r="AT45" s="86" t="s">
-        <v>232</v>
-      </c>
-      <c r="AU45" s="86" t="s">
-        <v>307</v>
-      </c>
-      <c r="AV45" s="86" t="s">
-        <v>300</v>
-      </c>
-      <c r="AW45" s="86" t="s">
+    </row>
+    <row r="49" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="AO49" s="76" t="s">
+        <v>149</v>
+      </c>
+      <c r="AP49" s="77">
+        <v>20</v>
+      </c>
+      <c r="AQ49" s="77">
+        <v>30</v>
+      </c>
+      <c r="AR49" s="77" t="s">
+        <v>59</v>
+      </c>
+      <c r="AS49" s="77" t="s">
+        <v>277</v>
+      </c>
+      <c r="AT49" s="77" t="s">
         <v>286</v>
       </c>
-    </row>
-    <row r="46" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="AO46" s="85" t="s">
-        <v>150</v>
-      </c>
-      <c r="AP46" s="86">
-        <v>22</v>
-      </c>
-      <c r="AQ46" s="86">
+      <c r="AU49" s="77" t="s">
+        <v>303</v>
+      </c>
+      <c r="AV49" s="77" t="s">
+        <v>296</v>
+      </c>
+      <c r="AW49" s="77" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="50" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="AO50" s="76" t="s">
+        <v>154</v>
+      </c>
+      <c r="AP50" s="77">
+        <v>19</v>
+      </c>
+      <c r="AQ50" s="77">
         <v>30</v>
       </c>
-      <c r="AR46" s="86" t="s">
+      <c r="AR50" s="77" t="s">
         <v>59</v>
       </c>
-      <c r="AS46" s="86" t="s">
-        <v>285</v>
-      </c>
-      <c r="AT46" s="86" t="s">
-        <v>287</v>
-      </c>
-      <c r="AU46" s="86" t="s">
-        <v>308</v>
-      </c>
-      <c r="AV46" s="86" t="s">
-        <v>301</v>
-      </c>
-      <c r="AW46" s="86" t="s">
+      <c r="AS50" s="77" t="s">
+        <v>277</v>
+      </c>
+      <c r="AT50" s="77" t="s">
         <v>288</v>
       </c>
-    </row>
-    <row r="47" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="AO47" s="85" t="s">
+      <c r="AU50" s="77" t="s">
+        <v>304</v>
+      </c>
+      <c r="AV50" s="77" t="s">
+        <v>297</v>
+      </c>
+      <c r="AW50" s="77" t="s">
         <v>289</v>
-      </c>
-      <c r="AP47" s="86">
-        <v>21</v>
-      </c>
-      <c r="AQ47" s="86">
-        <v>30</v>
-      </c>
-      <c r="AR47" s="86" t="s">
-        <v>59</v>
-      </c>
-      <c r="AS47" s="86" t="s">
-        <v>285</v>
-      </c>
-      <c r="AT47" s="86" t="s">
-        <v>290</v>
-      </c>
-      <c r="AU47" s="86" t="s">
-        <v>309</v>
-      </c>
-      <c r="AV47" s="86" t="s">
-        <v>302</v>
-      </c>
-      <c r="AW47" s="86" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="48" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="AO48" s="85" t="s">
-        <v>153</v>
-      </c>
-      <c r="AP48" s="86">
-        <v>20</v>
-      </c>
-      <c r="AQ48" s="86">
-        <v>30</v>
-      </c>
-      <c r="AR48" s="86" t="s">
-        <v>59</v>
-      </c>
-      <c r="AS48" s="86" t="s">
-        <v>285</v>
-      </c>
-      <c r="AT48" s="86" t="s">
-        <v>292</v>
-      </c>
-      <c r="AU48" s="86" t="s">
-        <v>310</v>
-      </c>
-      <c r="AV48" s="86" t="s">
-        <v>303</v>
-      </c>
-      <c r="AW48" s="86" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="49" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="AO49" s="85" t="s">
-        <v>149</v>
-      </c>
-      <c r="AP49" s="86">
-        <v>20</v>
-      </c>
-      <c r="AQ49" s="86">
-        <v>30</v>
-      </c>
-      <c r="AR49" s="86" t="s">
-        <v>59</v>
-      </c>
-      <c r="AS49" s="86" t="s">
-        <v>285</v>
-      </c>
-      <c r="AT49" s="86" t="s">
-        <v>294</v>
-      </c>
-      <c r="AU49" s="86" t="s">
-        <v>311</v>
-      </c>
-      <c r="AV49" s="86" t="s">
-        <v>304</v>
-      </c>
-      <c r="AW49" s="86" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="50" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="AO50" s="85" t="s">
-        <v>154</v>
-      </c>
-      <c r="AP50" s="86">
-        <v>19</v>
-      </c>
-      <c r="AQ50" s="86">
-        <v>30</v>
-      </c>
-      <c r="AR50" s="86" t="s">
-        <v>59</v>
-      </c>
-      <c r="AS50" s="86" t="s">
-        <v>285</v>
-      </c>
-      <c r="AT50" s="86" t="s">
-        <v>296</v>
-      </c>
-      <c r="AU50" s="86" t="s">
-        <v>312</v>
-      </c>
-      <c r="AV50" s="86" t="s">
-        <v>305</v>
-      </c>
-      <c r="AW50" s="86" t="s">
-        <v>297</v>
       </c>
     </row>
     <row r="51" spans="1:50" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3752,32 +3834,32 @@
       <c r="C51" s="6"/>
       <c r="D51" s="6"/>
       <c r="E51" s="6"/>
-      <c r="AO51" s="87" t="s">
+      <c r="AO51" s="78" t="s">
         <v>152</v>
       </c>
-      <c r="AP51" s="88">
+      <c r="AP51" s="79">
         <v>18</v>
       </c>
-      <c r="AQ51" s="88">
+      <c r="AQ51" s="79">
         <v>30</v>
       </c>
-      <c r="AR51" s="88" t="s">
+      <c r="AR51" s="79" t="s">
         <v>59</v>
       </c>
-      <c r="AS51" s="88" t="s">
-        <v>285</v>
-      </c>
-      <c r="AT51" s="88" t="s">
+      <c r="AS51" s="79" t="s">
+        <v>277</v>
+      </c>
+      <c r="AT51" s="79" t="s">
+        <v>290</v>
+      </c>
+      <c r="AU51" s="79" t="s">
+        <v>305</v>
+      </c>
+      <c r="AV51" s="79" t="s">
         <v>298</v>
       </c>
-      <c r="AU51" s="88" t="s">
-        <v>313</v>
-      </c>
-      <c r="AV51" s="88" t="s">
-        <v>306</v>
-      </c>
-      <c r="AW51" s="88" t="s">
-        <v>299</v>
+      <c r="AW51" s="79" t="s">
+        <v>291</v>
       </c>
     </row>
     <row r="52" spans="1:50" x14ac:dyDescent="0.25">
@@ -3797,7 +3879,15 @@
       <c r="G53" s="6"/>
       <c r="H53" s="6"/>
       <c r="I53" s="6"/>
-      <c r="AS53" s="1"/>
+      <c r="AO53" s="108" t="s">
+        <v>395</v>
+      </c>
+      <c r="AR53" s="62"/>
+      <c r="AS53" s="62"/>
+      <c r="AT53" s="62"/>
+      <c r="AU53" s="62"/>
+      <c r="AV53" s="62"/>
+      <c r="AW53" s="62"/>
     </row>
     <row r="54" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A54" s="6"/>
@@ -3809,8 +3899,11 @@
       <c r="G54" s="6"/>
       <c r="H54" s="6"/>
       <c r="I54" s="6"/>
-      <c r="AO54" s="89" t="s">
-        <v>314</v>
+      <c r="AO54" t="s">
+        <v>114</v>
+      </c>
+      <c r="AP54" s="14">
+        <v>42</v>
       </c>
       <c r="AR54" s="62"/>
       <c r="AS54" s="62"/>
@@ -3830,19 +3923,13 @@
       <c r="H55" s="6"/>
       <c r="I55" s="6"/>
       <c r="AO55" t="s">
-        <v>114</v>
-      </c>
-      <c r="AP55" s="14">
-        <v>152</v>
-      </c>
-      <c r="AR55" s="62"/>
-      <c r="AS55" s="62"/>
-      <c r="AT55" s="62"/>
-      <c r="AU55" s="62"/>
-      <c r="AV55" s="62"/>
-      <c r="AW55" s="62"/>
-    </row>
-    <row r="56" spans="1:50" x14ac:dyDescent="0.25">
+        <v>115</v>
+      </c>
+      <c r="AP55" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="56" spans="1:50" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="6"/>
       <c r="B56" s="6"/>
       <c r="C56" s="6"/>
@@ -3853,10 +3940,13 @@
       <c r="H56" s="6"/>
       <c r="I56" s="6"/>
       <c r="AO56" t="s">
-        <v>115</v>
+        <v>103</v>
       </c>
       <c r="AP56" t="s">
-        <v>254</v>
+        <v>396</v>
+      </c>
+      <c r="AQ56" t="s">
+        <v>266</v>
       </c>
     </row>
     <row r="57" spans="1:50" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3869,17 +3959,35 @@
       <c r="G57" s="27"/>
       <c r="H57" s="27"/>
       <c r="I57" s="27"/>
-      <c r="AO57" t="s">
+      <c r="AO57" s="105" t="s">
+        <v>94</v>
+      </c>
+      <c r="AP57" s="106" t="s">
+        <v>95</v>
+      </c>
+      <c r="AQ57" s="106" t="s">
+        <v>96</v>
+      </c>
+      <c r="AR57" s="106" t="s">
         <v>103</v>
       </c>
-      <c r="AP57" t="s">
-        <v>117</v>
-      </c>
-      <c r="AQ57" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="58" spans="1:50" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AS57" s="106" t="s">
+        <v>102</v>
+      </c>
+      <c r="AT57" s="106" t="s">
+        <v>104</v>
+      </c>
+      <c r="AU57" s="106" t="s">
+        <v>101</v>
+      </c>
+      <c r="AV57" s="106" t="s">
+        <v>43</v>
+      </c>
+      <c r="AW57" s="107" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="58" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A58" s="6"/>
       <c r="B58" s="29"/>
       <c r="C58" s="29"/>
@@ -3889,32 +3997,32 @@
       <c r="G58" s="29"/>
       <c r="H58" s="29"/>
       <c r="I58" s="29"/>
-      <c r="AO58" s="63" t="s">
-        <v>94</v>
-      </c>
-      <c r="AP58" s="64" t="s">
-        <v>95</v>
-      </c>
-      <c r="AQ58" s="64" t="s">
-        <v>96</v>
-      </c>
-      <c r="AR58" s="64" t="s">
-        <v>103</v>
-      </c>
-      <c r="AS58" s="64" t="s">
-        <v>102</v>
-      </c>
-      <c r="AT58" s="64" t="s">
-        <v>104</v>
-      </c>
-      <c r="AU58" s="64" t="s">
-        <v>101</v>
-      </c>
-      <c r="AV58" s="64" t="s">
-        <v>43</v>
-      </c>
-      <c r="AW58" s="65" t="s">
-        <v>40</v>
+      <c r="AO58" s="99" t="s">
+        <v>397</v>
+      </c>
+      <c r="AP58" s="100">
+        <v>14</v>
+      </c>
+      <c r="AQ58" s="100">
+        <v>14</v>
+      </c>
+      <c r="AR58" s="100" t="s">
+        <v>245</v>
+      </c>
+      <c r="AS58" s="100" t="s">
+        <v>398</v>
+      </c>
+      <c r="AT58" s="100" t="s">
+        <v>375</v>
+      </c>
+      <c r="AU58" s="100" t="s">
+        <v>409</v>
+      </c>
+      <c r="AV58" s="100" t="s">
+        <v>406</v>
+      </c>
+      <c r="AW58" s="101" t="s">
+        <v>399</v>
       </c>
     </row>
     <row r="59" spans="1:50" x14ac:dyDescent="0.25">
@@ -3927,35 +4035,35 @@
       <c r="G59" s="29"/>
       <c r="H59" s="29"/>
       <c r="I59" s="29"/>
-      <c r="AO59" s="90" t="s">
-        <v>152</v>
-      </c>
-      <c r="AP59" s="91">
-        <v>24</v>
-      </c>
-      <c r="AQ59" s="91">
-        <v>30</v>
-      </c>
-      <c r="AR59" s="91" t="s">
-        <v>59</v>
-      </c>
-      <c r="AS59" s="91" t="s">
-        <v>285</v>
-      </c>
-      <c r="AT59" s="91" t="s">
-        <v>254</v>
-      </c>
-      <c r="AU59" s="91" t="s">
-        <v>256</v>
-      </c>
-      <c r="AV59" s="91" t="s">
-        <v>329</v>
-      </c>
-      <c r="AW59" s="92" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="60" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="AO59" s="99" t="s">
+        <v>400</v>
+      </c>
+      <c r="AP59" s="100">
+        <v>14</v>
+      </c>
+      <c r="AQ59" s="100">
+        <v>14</v>
+      </c>
+      <c r="AR59" s="100" t="s">
+        <v>401</v>
+      </c>
+      <c r="AS59" s="100" t="s">
+        <v>398</v>
+      </c>
+      <c r="AT59" s="100" t="s">
+        <v>375</v>
+      </c>
+      <c r="AU59" s="100" t="s">
+        <v>410</v>
+      </c>
+      <c r="AV59" s="100" t="s">
+        <v>407</v>
+      </c>
+      <c r="AW59" s="101" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="60" spans="1:50" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="6"/>
       <c r="B60" s="29"/>
       <c r="C60" s="29"/>
@@ -3965,32 +4073,32 @@
       <c r="G60" s="29"/>
       <c r="H60" s="29"/>
       <c r="I60" s="29"/>
-      <c r="AO60" s="93" t="s">
-        <v>154</v>
-      </c>
-      <c r="AP60" s="94">
-        <v>24</v>
-      </c>
-      <c r="AQ60" s="94">
-        <v>30</v>
-      </c>
-      <c r="AR60" s="94" t="s">
-        <v>59</v>
-      </c>
-      <c r="AS60" s="94" t="s">
-        <v>285</v>
-      </c>
-      <c r="AT60" s="94" t="s">
-        <v>317</v>
-      </c>
-      <c r="AU60" s="94" t="s">
-        <v>336</v>
-      </c>
-      <c r="AV60" s="94" t="s">
-        <v>330</v>
-      </c>
-      <c r="AW60" s="95" t="s">
-        <v>318</v>
+      <c r="AO60" s="102" t="s">
+        <v>403</v>
+      </c>
+      <c r="AP60" s="103">
+        <v>14</v>
+      </c>
+      <c r="AQ60" s="103">
+        <v>14</v>
+      </c>
+      <c r="AR60" s="103" t="s">
+        <v>404</v>
+      </c>
+      <c r="AS60" s="103" t="s">
+        <v>398</v>
+      </c>
+      <c r="AT60" s="103" t="s">
+        <v>375</v>
+      </c>
+      <c r="AU60" s="103" t="s">
+        <v>411</v>
+      </c>
+      <c r="AV60" s="103" t="s">
+        <v>408</v>
+      </c>
+      <c r="AW60" s="104" t="s">
+        <v>405</v>
       </c>
     </row>
     <row r="61" spans="1:50" x14ac:dyDescent="0.25">
@@ -4003,33 +4111,6 @@
       <c r="G61" s="29"/>
       <c r="H61" s="29"/>
       <c r="I61" s="29"/>
-      <c r="AO61" s="93" t="s">
-        <v>289</v>
-      </c>
-      <c r="AP61" s="94">
-        <v>23</v>
-      </c>
-      <c r="AQ61" s="94">
-        <v>30</v>
-      </c>
-      <c r="AR61" s="94" t="s">
-        <v>59</v>
-      </c>
-      <c r="AS61" s="94" t="s">
-        <v>285</v>
-      </c>
-      <c r="AT61" s="94" t="s">
-        <v>319</v>
-      </c>
-      <c r="AU61" s="94" t="s">
-        <v>337</v>
-      </c>
-      <c r="AV61" s="94" t="s">
-        <v>331</v>
-      </c>
-      <c r="AW61" s="95" t="s">
-        <v>320</v>
-      </c>
     </row>
     <row r="62" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A62" s="6"/>
@@ -4038,33 +4119,6 @@
       <c r="D62" s="6"/>
       <c r="E62" s="6"/>
       <c r="AN62" s="6"/>
-      <c r="AO62" s="93" t="s">
-        <v>151</v>
-      </c>
-      <c r="AP62" s="94">
-        <v>21</v>
-      </c>
-      <c r="AQ62" s="94">
-        <v>30</v>
-      </c>
-      <c r="AR62" s="94" t="s">
-        <v>59</v>
-      </c>
-      <c r="AS62" s="94" t="s">
-        <v>285</v>
-      </c>
-      <c r="AT62" s="94" t="s">
-        <v>321</v>
-      </c>
-      <c r="AU62" s="94" t="s">
-        <v>338</v>
-      </c>
-      <c r="AV62" s="94" t="s">
-        <v>332</v>
-      </c>
-      <c r="AW62" s="95" t="s">
-        <v>322</v>
-      </c>
       <c r="AX62" s="62"/>
     </row>
     <row r="63" spans="1:50" x14ac:dyDescent="0.25">
@@ -4074,33 +4128,15 @@
       <c r="D63" s="6"/>
       <c r="E63" s="6"/>
       <c r="AN63" s="6"/>
-      <c r="AO63" s="93" t="s">
-        <v>153</v>
-      </c>
-      <c r="AP63" s="94">
-        <v>20</v>
-      </c>
-      <c r="AQ63" s="94">
-        <v>30</v>
-      </c>
-      <c r="AR63" s="94" t="s">
-        <v>59</v>
-      </c>
-      <c r="AS63" s="94" t="s">
-        <v>285</v>
-      </c>
-      <c r="AT63" s="94" t="s">
-        <v>323</v>
-      </c>
-      <c r="AU63" s="94" t="s">
-        <v>339</v>
-      </c>
-      <c r="AV63" s="94" t="s">
-        <v>333</v>
-      </c>
-      <c r="AW63" s="95" t="s">
-        <v>324</v>
-      </c>
+      <c r="AO63" s="80" t="s">
+        <v>306</v>
+      </c>
+      <c r="AR63" s="62"/>
+      <c r="AS63" s="62"/>
+      <c r="AT63" s="62"/>
+      <c r="AU63" s="62"/>
+      <c r="AV63" s="62"/>
+      <c r="AW63" s="62"/>
       <c r="AX63" s="62"/>
     </row>
     <row r="64" spans="1:50" x14ac:dyDescent="0.25">
@@ -4114,36 +4150,21 @@
       <c r="H64" s="6"/>
       <c r="I64" s="6"/>
       <c r="AN64" s="6"/>
-      <c r="AO64" s="93" t="s">
-        <v>150</v>
-      </c>
-      <c r="AP64" s="94">
-        <v>20</v>
-      </c>
-      <c r="AQ64" s="94">
-        <v>30</v>
-      </c>
-      <c r="AR64" s="94" t="s">
-        <v>59</v>
-      </c>
-      <c r="AS64" s="94" t="s">
-        <v>285</v>
-      </c>
-      <c r="AT64" s="94" t="s">
-        <v>325</v>
-      </c>
-      <c r="AU64" s="94" t="s">
-        <v>340</v>
-      </c>
-      <c r="AV64" s="94" t="s">
-        <v>334</v>
-      </c>
-      <c r="AW64" s="95" t="s">
-        <v>326</v>
-      </c>
+      <c r="AO64" t="s">
+        <v>114</v>
+      </c>
+      <c r="AP64" s="14">
+        <v>152</v>
+      </c>
+      <c r="AR64" s="62"/>
+      <c r="AS64" s="62"/>
+      <c r="AT64" s="62"/>
+      <c r="AU64" s="62"/>
+      <c r="AV64" s="62"/>
+      <c r="AW64" s="62"/>
       <c r="AX64" s="62"/>
     </row>
-    <row r="65" spans="1:50" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A65" s="6"/>
       <c r="B65" s="30"/>
       <c r="C65" s="6"/>
@@ -4154,36 +4175,15 @@
       <c r="H65" s="6"/>
       <c r="I65" s="6"/>
       <c r="AN65" s="6"/>
-      <c r="AO65" s="96" t="s">
-        <v>149</v>
-      </c>
-      <c r="AP65" s="97">
-        <v>20</v>
-      </c>
-      <c r="AQ65" s="97">
-        <v>30</v>
-      </c>
-      <c r="AR65" s="97" t="s">
-        <v>59</v>
-      </c>
-      <c r="AS65" s="97" t="s">
-        <v>285</v>
-      </c>
-      <c r="AT65" s="97" t="s">
-        <v>327</v>
-      </c>
-      <c r="AU65" s="97" t="s">
-        <v>341</v>
-      </c>
-      <c r="AV65" s="97" t="s">
-        <v>335</v>
-      </c>
-      <c r="AW65" s="98" t="s">
-        <v>328</v>
+      <c r="AO65" t="s">
+        <v>115</v>
+      </c>
+      <c r="AP65" t="s">
+        <v>246</v>
       </c>
       <c r="AX65" s="62"/>
     </row>
-    <row r="66" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:50" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A66" s="6"/>
       <c r="B66" s="6"/>
       <c r="C66" s="6"/>
@@ -4194,18 +4194,18 @@
       <c r="H66" s="6"/>
       <c r="I66" s="6"/>
       <c r="AN66" s="6"/>
-      <c r="AO66" s="6"/>
-      <c r="AP66" s="6"/>
-      <c r="AQ66" s="6"/>
-      <c r="AR66" s="6"/>
-      <c r="AS66" s="6"/>
-      <c r="AT66" s="6"/>
-      <c r="AU66" s="6"/>
-      <c r="AV66" s="6"/>
-      <c r="AW66" s="6"/>
+      <c r="AO66" t="s">
+        <v>103</v>
+      </c>
+      <c r="AP66" t="s">
+        <v>117</v>
+      </c>
+      <c r="AQ66" t="s">
+        <v>116</v>
+      </c>
       <c r="AX66" s="62"/>
     </row>
-    <row r="67" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:50" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A67" s="6"/>
       <c r="B67" s="6"/>
       <c r="C67" s="6"/>
@@ -4216,14 +4216,33 @@
       <c r="H67" s="6"/>
       <c r="I67" s="6"/>
       <c r="AN67" s="2"/>
-      <c r="AO67" s="2"/>
-      <c r="AP67" s="2"/>
-      <c r="AQ67" s="2"/>
-      <c r="AS67" s="2"/>
-      <c r="AT67" s="2"/>
-      <c r="AU67" s="2"/>
-      <c r="AV67" s="2"/>
-      <c r="AW67" s="2"/>
+      <c r="AO67" s="63" t="s">
+        <v>94</v>
+      </c>
+      <c r="AP67" s="64" t="s">
+        <v>95</v>
+      </c>
+      <c r="AQ67" s="64" t="s">
+        <v>96</v>
+      </c>
+      <c r="AR67" s="64" t="s">
+        <v>103</v>
+      </c>
+      <c r="AS67" s="64" t="s">
+        <v>102</v>
+      </c>
+      <c r="AT67" s="64" t="s">
+        <v>104</v>
+      </c>
+      <c r="AU67" s="64" t="s">
+        <v>101</v>
+      </c>
+      <c r="AV67" s="64" t="s">
+        <v>43</v>
+      </c>
+      <c r="AW67" s="65" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="68" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A68" s="28"/>
@@ -4235,6 +4254,33 @@
       <c r="G68" s="27"/>
       <c r="H68" s="27"/>
       <c r="I68" s="27"/>
+      <c r="AO68" s="81" t="s">
+        <v>152</v>
+      </c>
+      <c r="AP68" s="82">
+        <v>24</v>
+      </c>
+      <c r="AQ68" s="82">
+        <v>30</v>
+      </c>
+      <c r="AR68" s="82" t="s">
+        <v>59</v>
+      </c>
+      <c r="AS68" s="82" t="s">
+        <v>277</v>
+      </c>
+      <c r="AT68" s="82" t="s">
+        <v>246</v>
+      </c>
+      <c r="AU68" s="82" t="s">
+        <v>248</v>
+      </c>
+      <c r="AV68" s="82" t="s">
+        <v>321</v>
+      </c>
+      <c r="AW68" s="83" t="s">
+        <v>308</v>
+      </c>
     </row>
     <row r="69" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A69" s="6"/>
@@ -4246,15 +4292,33 @@
       <c r="G69" s="29"/>
       <c r="H69" s="29"/>
       <c r="I69" s="29"/>
-      <c r="AO69" s="89" t="s">
-        <v>342</v>
-      </c>
-      <c r="AR69" s="62"/>
-      <c r="AS69" s="62"/>
-      <c r="AT69" s="62"/>
-      <c r="AU69" s="62"/>
-      <c r="AV69" s="62"/>
-      <c r="AW69" s="62"/>
+      <c r="AO69" s="84" t="s">
+        <v>154</v>
+      </c>
+      <c r="AP69" s="85">
+        <v>24</v>
+      </c>
+      <c r="AQ69" s="85">
+        <v>30</v>
+      </c>
+      <c r="AR69" s="85" t="s">
+        <v>59</v>
+      </c>
+      <c r="AS69" s="85" t="s">
+        <v>277</v>
+      </c>
+      <c r="AT69" s="85" t="s">
+        <v>309</v>
+      </c>
+      <c r="AU69" s="85" t="s">
+        <v>328</v>
+      </c>
+      <c r="AV69" s="85" t="s">
+        <v>322</v>
+      </c>
+      <c r="AW69" s="86" t="s">
+        <v>310</v>
+      </c>
     </row>
     <row r="70" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A70" s="6"/>
@@ -4266,18 +4330,33 @@
       <c r="G70" s="29"/>
       <c r="H70" s="29"/>
       <c r="I70" s="29"/>
-      <c r="AO70" t="s">
-        <v>114</v>
-      </c>
-      <c r="AP70" s="14">
-        <v>146</v>
-      </c>
-      <c r="AR70" s="62"/>
-      <c r="AS70" s="62"/>
-      <c r="AT70" s="62"/>
-      <c r="AU70" s="62"/>
-      <c r="AV70" s="62"/>
-      <c r="AW70" s="62"/>
+      <c r="AO70" s="84" t="s">
+        <v>281</v>
+      </c>
+      <c r="AP70" s="85">
+        <v>23</v>
+      </c>
+      <c r="AQ70" s="85">
+        <v>30</v>
+      </c>
+      <c r="AR70" s="85" t="s">
+        <v>59</v>
+      </c>
+      <c r="AS70" s="85" t="s">
+        <v>277</v>
+      </c>
+      <c r="AT70" s="85" t="s">
+        <v>311</v>
+      </c>
+      <c r="AU70" s="85" t="s">
+        <v>329</v>
+      </c>
+      <c r="AV70" s="85" t="s">
+        <v>323</v>
+      </c>
+      <c r="AW70" s="86" t="s">
+        <v>312</v>
+      </c>
     </row>
     <row r="71" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A71" s="6"/>
@@ -4289,14 +4368,35 @@
       <c r="G71" s="29"/>
       <c r="H71" s="29"/>
       <c r="I71" s="29"/>
-      <c r="AO71" t="s">
-        <v>115</v>
-      </c>
-      <c r="AP71" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="72" spans="1:50" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AO71" s="84" t="s">
+        <v>151</v>
+      </c>
+      <c r="AP71" s="85">
+        <v>21</v>
+      </c>
+      <c r="AQ71" s="85">
+        <v>30</v>
+      </c>
+      <c r="AR71" s="85" t="s">
+        <v>59</v>
+      </c>
+      <c r="AS71" s="85" t="s">
+        <v>277</v>
+      </c>
+      <c r="AT71" s="85" t="s">
+        <v>313</v>
+      </c>
+      <c r="AU71" s="85" t="s">
+        <v>330</v>
+      </c>
+      <c r="AV71" s="85" t="s">
+        <v>324</v>
+      </c>
+      <c r="AW71" s="86" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="72" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A72" s="6"/>
       <c r="B72" s="29"/>
       <c r="C72" s="29"/>
@@ -4306,82 +4406,100 @@
       <c r="G72" s="29"/>
       <c r="H72" s="29"/>
       <c r="I72" s="29"/>
-      <c r="AO72" t="s">
-        <v>103</v>
-      </c>
-      <c r="AP72" t="s">
-        <v>117</v>
-      </c>
-      <c r="AQ72" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="73" spans="1:50" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AO72" s="84" t="s">
+        <v>153</v>
+      </c>
+      <c r="AP72" s="85">
+        <v>20</v>
+      </c>
+      <c r="AQ72" s="85">
+        <v>30</v>
+      </c>
+      <c r="AR72" s="85" t="s">
+        <v>59</v>
+      </c>
+      <c r="AS72" s="85" t="s">
+        <v>277</v>
+      </c>
+      <c r="AT72" s="85" t="s">
+        <v>315</v>
+      </c>
+      <c r="AU72" s="85" t="s">
+        <v>331</v>
+      </c>
+      <c r="AV72" s="85" t="s">
+        <v>325</v>
+      </c>
+      <c r="AW72" s="86" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="73" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A73" s="6"/>
       <c r="B73" s="6"/>
       <c r="C73" s="6"/>
       <c r="D73" s="6"/>
       <c r="E73" s="6"/>
-      <c r="AO73" s="63" t="s">
-        <v>94</v>
-      </c>
-      <c r="AP73" s="64" t="s">
-        <v>95</v>
-      </c>
-      <c r="AQ73" s="64" t="s">
-        <v>96</v>
-      </c>
-      <c r="AR73" s="64" t="s">
-        <v>103</v>
-      </c>
-      <c r="AS73" s="64" t="s">
-        <v>102</v>
-      </c>
-      <c r="AT73" s="64" t="s">
-        <v>104</v>
-      </c>
-      <c r="AU73" s="64" t="s">
-        <v>101</v>
-      </c>
-      <c r="AV73" s="64" t="s">
-        <v>43</v>
-      </c>
-      <c r="AW73" s="65" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="74" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="AO73" s="84" t="s">
+        <v>150</v>
+      </c>
+      <c r="AP73" s="85">
+        <v>20</v>
+      </c>
+      <c r="AQ73" s="85">
+        <v>30</v>
+      </c>
+      <c r="AR73" s="85" t="s">
+        <v>59</v>
+      </c>
+      <c r="AS73" s="85" t="s">
+        <v>277</v>
+      </c>
+      <c r="AT73" s="85" t="s">
+        <v>317</v>
+      </c>
+      <c r="AU73" s="85" t="s">
+        <v>332</v>
+      </c>
+      <c r="AV73" s="85" t="s">
+        <v>326</v>
+      </c>
+      <c r="AW73" s="86" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="74" spans="1:50" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A74" s="6"/>
       <c r="B74" s="6"/>
       <c r="C74" s="6"/>
       <c r="D74" s="6"/>
       <c r="E74" s="6"/>
-      <c r="AO74" s="90" t="s">
-        <v>151</v>
-      </c>
-      <c r="AP74" s="91">
-        <v>24</v>
-      </c>
-      <c r="AQ74" s="91">
+      <c r="AO74" s="87" t="s">
+        <v>149</v>
+      </c>
+      <c r="AP74" s="88">
+        <v>20</v>
+      </c>
+      <c r="AQ74" s="88">
         <v>30</v>
       </c>
-      <c r="AR74" s="91" t="s">
+      <c r="AR74" s="88" t="s">
         <v>59</v>
       </c>
-      <c r="AS74" s="91" t="s">
-        <v>285</v>
-      </c>
-      <c r="AT74" s="91" t="s">
-        <v>255</v>
-      </c>
-      <c r="AU74" s="91" t="s">
-        <v>257</v>
-      </c>
-      <c r="AV74" s="91" t="s">
-        <v>356</v>
-      </c>
-      <c r="AW74" s="92" t="s">
-        <v>343</v>
+      <c r="AS74" s="88" t="s">
+        <v>277</v>
+      </c>
+      <c r="AT74" s="88" t="s">
+        <v>319</v>
+      </c>
+      <c r="AU74" s="88" t="s">
+        <v>333</v>
+      </c>
+      <c r="AV74" s="88" t="s">
+        <v>327</v>
+      </c>
+      <c r="AW74" s="89" t="s">
+        <v>320</v>
       </c>
     </row>
     <row r="75" spans="1:50" x14ac:dyDescent="0.25">
@@ -4390,33 +4508,15 @@
       <c r="C75" s="6"/>
       <c r="D75" s="6"/>
       <c r="E75" s="6"/>
-      <c r="AO75" s="93" t="s">
-        <v>289</v>
-      </c>
-      <c r="AP75" s="94">
-        <v>23</v>
-      </c>
-      <c r="AQ75" s="94">
-        <v>30</v>
-      </c>
-      <c r="AR75" s="94" t="s">
-        <v>59</v>
-      </c>
-      <c r="AS75" s="94" t="s">
-        <v>285</v>
-      </c>
-      <c r="AT75" s="94" t="s">
-        <v>344</v>
-      </c>
-      <c r="AU75" s="94" t="s">
-        <v>363</v>
-      </c>
-      <c r="AV75" s="94" t="s">
-        <v>357</v>
-      </c>
-      <c r="AW75" s="95" t="s">
-        <v>345</v>
-      </c>
+      <c r="AO75" s="6"/>
+      <c r="AP75" s="6"/>
+      <c r="AQ75" s="6"/>
+      <c r="AR75" s="6"/>
+      <c r="AS75" s="6"/>
+      <c r="AT75" s="6"/>
+      <c r="AU75" s="6"/>
+      <c r="AV75" s="6"/>
+      <c r="AW75" s="6"/>
     </row>
     <row r="76" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A76" s="6"/>
@@ -4424,33 +4524,14 @@
       <c r="C76" s="6"/>
       <c r="D76" s="6"/>
       <c r="E76" s="6"/>
-      <c r="AO76" s="93" t="s">
-        <v>150</v>
-      </c>
-      <c r="AP76" s="94">
-        <v>22</v>
-      </c>
-      <c r="AQ76" s="94">
-        <v>30</v>
-      </c>
-      <c r="AR76" s="94" t="s">
-        <v>59</v>
-      </c>
-      <c r="AS76" s="94" t="s">
-        <v>285</v>
-      </c>
-      <c r="AT76" s="94" t="s">
-        <v>346</v>
-      </c>
-      <c r="AU76" s="94" t="s">
-        <v>364</v>
-      </c>
-      <c r="AV76" s="94" t="s">
-        <v>358</v>
-      </c>
-      <c r="AW76" s="95" t="s">
-        <v>347</v>
-      </c>
+      <c r="AO76" s="2"/>
+      <c r="AP76" s="2"/>
+      <c r="AQ76" s="2"/>
+      <c r="AS76" s="2"/>
+      <c r="AT76" s="2"/>
+      <c r="AU76" s="2"/>
+      <c r="AV76" s="2"/>
+      <c r="AW76" s="2"/>
     </row>
     <row r="77" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A77" s="6"/>
@@ -4458,33 +4539,6 @@
       <c r="C77" s="6"/>
       <c r="D77" s="6"/>
       <c r="E77" s="6"/>
-      <c r="AO77" s="93" t="s">
-        <v>153</v>
-      </c>
-      <c r="AP77" s="94">
-        <v>20</v>
-      </c>
-      <c r="AQ77" s="94">
-        <v>30</v>
-      </c>
-      <c r="AR77" s="94" t="s">
-        <v>59</v>
-      </c>
-      <c r="AS77" s="94" t="s">
-        <v>285</v>
-      </c>
-      <c r="AT77" s="94" t="s">
-        <v>348</v>
-      </c>
-      <c r="AU77" s="94" t="s">
-        <v>365</v>
-      </c>
-      <c r="AV77" s="94" t="s">
-        <v>359</v>
-      </c>
-      <c r="AW77" s="95" t="s">
-        <v>349</v>
-      </c>
     </row>
     <row r="78" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A78" s="6"/>
@@ -4492,33 +4546,15 @@
       <c r="C78" s="6"/>
       <c r="D78" s="6"/>
       <c r="E78" s="6"/>
-      <c r="AO78" s="93" t="s">
-        <v>149</v>
-      </c>
-      <c r="AP78" s="94">
-        <v>20</v>
-      </c>
-      <c r="AQ78" s="94">
-        <v>30</v>
-      </c>
-      <c r="AR78" s="94" t="s">
-        <v>59</v>
-      </c>
-      <c r="AS78" s="94" t="s">
-        <v>285</v>
-      </c>
-      <c r="AT78" s="94" t="s">
-        <v>350</v>
-      </c>
-      <c r="AU78" s="94" t="s">
-        <v>366</v>
-      </c>
-      <c r="AV78" s="94" t="s">
-        <v>360</v>
-      </c>
-      <c r="AW78" s="95" t="s">
-        <v>351</v>
-      </c>
+      <c r="AO78" s="80" t="s">
+        <v>334</v>
+      </c>
+      <c r="AR78" s="62"/>
+      <c r="AS78" s="62"/>
+      <c r="AT78" s="62"/>
+      <c r="AU78" s="62"/>
+      <c r="AV78" s="62"/>
+      <c r="AW78" s="62"/>
     </row>
     <row r="79" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A79" s="6"/>
@@ -4526,81 +4562,81 @@
       <c r="C79" s="6"/>
       <c r="D79" s="6"/>
       <c r="E79" s="6"/>
-      <c r="AO79" s="93" t="s">
-        <v>154</v>
-      </c>
-      <c r="AP79" s="94">
-        <v>19</v>
-      </c>
-      <c r="AQ79" s="94">
-        <v>30</v>
-      </c>
-      <c r="AR79" s="94" t="s">
-        <v>59</v>
-      </c>
-      <c r="AS79" s="94" t="s">
-        <v>285</v>
-      </c>
-      <c r="AT79" s="94" t="s">
-        <v>352</v>
-      </c>
-      <c r="AU79" s="94" t="s">
-        <v>367</v>
-      </c>
-      <c r="AV79" s="94" t="s">
-        <v>361</v>
-      </c>
-      <c r="AW79" s="95" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="80" spans="1:50" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AO79" t="s">
+        <v>114</v>
+      </c>
+      <c r="AP79" s="14">
+        <v>146</v>
+      </c>
+      <c r="AR79" s="62"/>
+      <c r="AS79" s="62"/>
+      <c r="AT79" s="62"/>
+      <c r="AU79" s="62"/>
+      <c r="AV79" s="62"/>
+      <c r="AW79" s="62"/>
+    </row>
+    <row r="80" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A80" s="6"/>
       <c r="B80" s="6"/>
       <c r="C80" s="6"/>
       <c r="D80" s="6"/>
       <c r="E80" s="6"/>
-      <c r="AO80" s="96" t="s">
-        <v>152</v>
-      </c>
-      <c r="AP80" s="97">
-        <v>18</v>
-      </c>
-      <c r="AQ80" s="97">
-        <v>30</v>
-      </c>
-      <c r="AR80" s="97" t="s">
-        <v>59</v>
-      </c>
-      <c r="AS80" s="97" t="s">
-        <v>285</v>
-      </c>
-      <c r="AT80" s="97" t="s">
-        <v>354</v>
-      </c>
-      <c r="AU80" s="97" t="s">
-        <v>368</v>
-      </c>
-      <c r="AV80" s="97" t="s">
-        <v>362</v>
-      </c>
-      <c r="AW80" s="98" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="81" spans="1:49" x14ac:dyDescent="0.25">
+      <c r="AO80" t="s">
+        <v>115</v>
+      </c>
+      <c r="AP80" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="81" spans="1:49" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A81" s="6"/>
       <c r="B81" s="6"/>
       <c r="C81" s="6"/>
       <c r="D81" s="6"/>
       <c r="E81" s="6"/>
-    </row>
-    <row r="82" spans="1:49" x14ac:dyDescent="0.25">
+      <c r="AO81" t="s">
+        <v>103</v>
+      </c>
+      <c r="AP81" t="s">
+        <v>117</v>
+      </c>
+      <c r="AQ81" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="82" spans="1:49" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A82" s="6"/>
       <c r="B82" s="6"/>
       <c r="C82" s="6"/>
       <c r="D82" s="6"/>
       <c r="E82" s="6"/>
+      <c r="AO82" s="63" t="s">
+        <v>94</v>
+      </c>
+      <c r="AP82" s="64" t="s">
+        <v>95</v>
+      </c>
+      <c r="AQ82" s="64" t="s">
+        <v>96</v>
+      </c>
+      <c r="AR82" s="64" t="s">
+        <v>103</v>
+      </c>
+      <c r="AS82" s="64" t="s">
+        <v>102</v>
+      </c>
+      <c r="AT82" s="64" t="s">
+        <v>104</v>
+      </c>
+      <c r="AU82" s="64" t="s">
+        <v>101</v>
+      </c>
+      <c r="AV82" s="64" t="s">
+        <v>43</v>
+      </c>
+      <c r="AW82" s="65" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="83" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A83" s="6"/>
@@ -4608,15 +4644,33 @@
       <c r="C83" s="6"/>
       <c r="D83" s="6"/>
       <c r="E83" s="6"/>
-      <c r="AO83" s="89" t="s">
-        <v>369</v>
-      </c>
-      <c r="AR83" s="62"/>
-      <c r="AS83" s="62"/>
-      <c r="AT83" s="62"/>
-      <c r="AU83" s="62"/>
-      <c r="AV83" s="62"/>
-      <c r="AW83" s="62"/>
+      <c r="AO83" s="81" t="s">
+        <v>151</v>
+      </c>
+      <c r="AP83" s="82">
+        <v>24</v>
+      </c>
+      <c r="AQ83" s="82">
+        <v>30</v>
+      </c>
+      <c r="AR83" s="82" t="s">
+        <v>59</v>
+      </c>
+      <c r="AS83" s="82" t="s">
+        <v>277</v>
+      </c>
+      <c r="AT83" s="82" t="s">
+        <v>247</v>
+      </c>
+      <c r="AU83" s="82" t="s">
+        <v>249</v>
+      </c>
+      <c r="AV83" s="82" t="s">
+        <v>348</v>
+      </c>
+      <c r="AW83" s="83" t="s">
+        <v>335</v>
+      </c>
     </row>
     <row r="84" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A84" s="6"/>
@@ -4624,18 +4678,33 @@
       <c r="C84" s="6"/>
       <c r="D84" s="6"/>
       <c r="E84" s="6"/>
-      <c r="AO84" t="s">
-        <v>114</v>
-      </c>
-      <c r="AP84" s="14">
-        <v>138</v>
-      </c>
-      <c r="AR84" s="62"/>
-      <c r="AS84" s="62"/>
-      <c r="AT84" s="62"/>
-      <c r="AU84" s="62"/>
-      <c r="AV84" s="62"/>
-      <c r="AW84" s="62"/>
+      <c r="AO84" s="84" t="s">
+        <v>281</v>
+      </c>
+      <c r="AP84" s="85">
+        <v>23</v>
+      </c>
+      <c r="AQ84" s="85">
+        <v>30</v>
+      </c>
+      <c r="AR84" s="85" t="s">
+        <v>59</v>
+      </c>
+      <c r="AS84" s="85" t="s">
+        <v>277</v>
+      </c>
+      <c r="AT84" s="85" t="s">
+        <v>336</v>
+      </c>
+      <c r="AU84" s="85" t="s">
+        <v>355</v>
+      </c>
+      <c r="AV84" s="85" t="s">
+        <v>349</v>
+      </c>
+      <c r="AW84" s="86" t="s">
+        <v>337</v>
+      </c>
     </row>
     <row r="85" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A85" s="6"/>
@@ -4643,61 +4712,100 @@
       <c r="C85" s="6"/>
       <c r="D85" s="6"/>
       <c r="E85" s="6"/>
-      <c r="AO85" t="s">
-        <v>115</v>
-      </c>
-      <c r="AP85" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="86" spans="1:49" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AO85" s="84" t="s">
+        <v>150</v>
+      </c>
+      <c r="AP85" s="85">
+        <v>22</v>
+      </c>
+      <c r="AQ85" s="85">
+        <v>30</v>
+      </c>
+      <c r="AR85" s="85" t="s">
+        <v>59</v>
+      </c>
+      <c r="AS85" s="85" t="s">
+        <v>277</v>
+      </c>
+      <c r="AT85" s="85" t="s">
+        <v>338</v>
+      </c>
+      <c r="AU85" s="85" t="s">
+        <v>356</v>
+      </c>
+      <c r="AV85" s="85" t="s">
+        <v>350</v>
+      </c>
+      <c r="AW85" s="86" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="86" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A86" s="6"/>
       <c r="B86" s="6"/>
       <c r="C86" s="6"/>
       <c r="D86" s="6"/>
       <c r="E86" s="6"/>
-      <c r="AO86" t="s">
-        <v>103</v>
-      </c>
-      <c r="AP86" t="s">
-        <v>117</v>
-      </c>
-      <c r="AQ86" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="87" spans="1:49" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AO86" s="84" t="s">
+        <v>153</v>
+      </c>
+      <c r="AP86" s="85">
+        <v>20</v>
+      </c>
+      <c r="AQ86" s="85">
+        <v>30</v>
+      </c>
+      <c r="AR86" s="85" t="s">
+        <v>59</v>
+      </c>
+      <c r="AS86" s="85" t="s">
+        <v>277</v>
+      </c>
+      <c r="AT86" s="85" t="s">
+        <v>340</v>
+      </c>
+      <c r="AU86" s="85" t="s">
+        <v>357</v>
+      </c>
+      <c r="AV86" s="85" t="s">
+        <v>351</v>
+      </c>
+      <c r="AW86" s="86" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="87" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A87" s="6"/>
       <c r="B87" s="6"/>
       <c r="C87" s="6"/>
       <c r="D87" s="6"/>
       <c r="E87" s="6"/>
-      <c r="AO87" s="63" t="s">
-        <v>94</v>
-      </c>
-      <c r="AP87" s="64" t="s">
-        <v>95</v>
-      </c>
-      <c r="AQ87" s="64" t="s">
-        <v>96</v>
-      </c>
-      <c r="AR87" s="64" t="s">
-        <v>103</v>
-      </c>
-      <c r="AS87" s="64" t="s">
-        <v>102</v>
-      </c>
-      <c r="AT87" s="64" t="s">
-        <v>104</v>
-      </c>
-      <c r="AU87" s="64" t="s">
-        <v>101</v>
-      </c>
-      <c r="AV87" s="64" t="s">
-        <v>43</v>
-      </c>
-      <c r="AW87" s="65" t="s">
-        <v>40</v>
+      <c r="AO87" s="84" t="s">
+        <v>149</v>
+      </c>
+      <c r="AP87" s="85">
+        <v>20</v>
+      </c>
+      <c r="AQ87" s="85">
+        <v>30</v>
+      </c>
+      <c r="AR87" s="85" t="s">
+        <v>59</v>
+      </c>
+      <c r="AS87" s="85" t="s">
+        <v>277</v>
+      </c>
+      <c r="AT87" s="85" t="s">
+        <v>342</v>
+      </c>
+      <c r="AU87" s="85" t="s">
+        <v>358</v>
+      </c>
+      <c r="AV87" s="85" t="s">
+        <v>352</v>
+      </c>
+      <c r="AW87" s="86" t="s">
+        <v>343</v>
       </c>
     </row>
     <row r="88" spans="1:49" x14ac:dyDescent="0.25">
@@ -4706,66 +4814,66 @@
       <c r="C88" s="6"/>
       <c r="D88" s="6"/>
       <c r="E88" s="6"/>
-      <c r="AO88" s="90" t="s">
-        <v>153</v>
-      </c>
-      <c r="AP88" s="91">
-        <v>24</v>
-      </c>
-      <c r="AQ88" s="91">
+      <c r="AO88" s="84" t="s">
+        <v>154</v>
+      </c>
+      <c r="AP88" s="85">
+        <v>19</v>
+      </c>
+      <c r="AQ88" s="85">
         <v>30</v>
       </c>
-      <c r="AR88" s="91" t="s">
-        <v>315</v>
-      </c>
-      <c r="AS88" s="91" t="s">
-        <v>285</v>
-      </c>
-      <c r="AT88" s="91" t="s">
+      <c r="AR88" s="85" t="s">
         <v>59</v>
       </c>
-      <c r="AU88" s="91" t="s">
-        <v>268</v>
-      </c>
-      <c r="AV88" s="91" t="s">
-        <v>385</v>
-      </c>
-      <c r="AW88" s="92" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="89" spans="1:49" x14ac:dyDescent="0.25">
+      <c r="AS88" s="85" t="s">
+        <v>277</v>
+      </c>
+      <c r="AT88" s="85" t="s">
+        <v>344</v>
+      </c>
+      <c r="AU88" s="85" t="s">
+        <v>359</v>
+      </c>
+      <c r="AV88" s="85" t="s">
+        <v>353</v>
+      </c>
+      <c r="AW88" s="86" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="89" spans="1:49" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A89" s="6"/>
       <c r="B89" s="6"/>
       <c r="C89" s="6"/>
       <c r="D89" s="6"/>
       <c r="E89" s="6"/>
-      <c r="AO89" s="93" t="s">
-        <v>154</v>
-      </c>
-      <c r="AP89" s="94">
-        <v>23</v>
-      </c>
-      <c r="AQ89" s="94">
+      <c r="AO89" s="87" t="s">
+        <v>152</v>
+      </c>
+      <c r="AP89" s="88">
+        <v>18</v>
+      </c>
+      <c r="AQ89" s="88">
         <v>30</v>
       </c>
-      <c r="AR89" s="94" t="s">
-        <v>371</v>
-      </c>
-      <c r="AS89" s="94" t="s">
-        <v>285</v>
-      </c>
-      <c r="AT89" s="94" t="s">
+      <c r="AR89" s="88" t="s">
         <v>59</v>
       </c>
-      <c r="AU89" s="94" t="s">
-        <v>390</v>
-      </c>
-      <c r="AV89" s="94" t="s">
-        <v>389</v>
-      </c>
-      <c r="AW89" s="95" t="s">
-        <v>372</v>
+      <c r="AS89" s="88" t="s">
+        <v>277</v>
+      </c>
+      <c r="AT89" s="88" t="s">
+        <v>346</v>
+      </c>
+      <c r="AU89" s="88" t="s">
+        <v>360</v>
+      </c>
+      <c r="AV89" s="88" t="s">
+        <v>354</v>
+      </c>
+      <c r="AW89" s="89" t="s">
+        <v>347</v>
       </c>
     </row>
     <row r="90" spans="1:49" x14ac:dyDescent="0.25">
@@ -4774,33 +4882,6 @@
       <c r="C90" s="6"/>
       <c r="D90" s="6"/>
       <c r="E90" s="6"/>
-      <c r="AO90" s="93" t="s">
-        <v>149</v>
-      </c>
-      <c r="AP90" s="94">
-        <v>23</v>
-      </c>
-      <c r="AQ90" s="94">
-        <v>30</v>
-      </c>
-      <c r="AR90" s="94" t="s">
-        <v>373</v>
-      </c>
-      <c r="AS90" s="94" t="s">
-        <v>285</v>
-      </c>
-      <c r="AT90" s="94" t="s">
-        <v>59</v>
-      </c>
-      <c r="AU90" s="94" t="s">
-        <v>391</v>
-      </c>
-      <c r="AV90" s="94" t="s">
-        <v>372</v>
-      </c>
-      <c r="AW90" s="95" t="s">
-        <v>374</v>
-      </c>
     </row>
     <row r="91" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A91" s="6"/>
@@ -4808,33 +4889,6 @@
       <c r="C91" s="6"/>
       <c r="D91" s="6"/>
       <c r="E91" s="6"/>
-      <c r="AO91" s="93" t="s">
-        <v>151</v>
-      </c>
-      <c r="AP91" s="94">
-        <v>20</v>
-      </c>
-      <c r="AQ91" s="94">
-        <v>30</v>
-      </c>
-      <c r="AR91" s="94" t="s">
-        <v>375</v>
-      </c>
-      <c r="AS91" s="94" t="s">
-        <v>285</v>
-      </c>
-      <c r="AT91" s="94" t="s">
-        <v>59</v>
-      </c>
-      <c r="AU91" s="94" t="s">
-        <v>392</v>
-      </c>
-      <c r="AV91" s="94" t="s">
-        <v>373</v>
-      </c>
-      <c r="AW91" s="95" t="s">
-        <v>376</v>
-      </c>
     </row>
     <row r="92" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A92" s="6"/>
@@ -4842,33 +4896,15 @@
       <c r="C92" s="6"/>
       <c r="D92" s="6"/>
       <c r="E92" s="6"/>
-      <c r="AO92" s="93" t="s">
-        <v>289</v>
-      </c>
-      <c r="AP92" s="94">
-        <v>18</v>
-      </c>
-      <c r="AQ92" s="94">
-        <v>30</v>
-      </c>
-      <c r="AR92" s="94" t="s">
-        <v>377</v>
-      </c>
-      <c r="AS92" s="94" t="s">
-        <v>285</v>
-      </c>
-      <c r="AT92" s="94" t="s">
-        <v>59</v>
-      </c>
-      <c r="AU92" s="94" t="s">
-        <v>393</v>
-      </c>
-      <c r="AV92" s="94" t="s">
-        <v>386</v>
-      </c>
-      <c r="AW92" s="95" t="s">
-        <v>378</v>
-      </c>
+      <c r="AO92" s="80" t="s">
+        <v>361</v>
+      </c>
+      <c r="AR92" s="62"/>
+      <c r="AS92" s="62"/>
+      <c r="AT92" s="62"/>
+      <c r="AU92" s="62"/>
+      <c r="AV92" s="62"/>
+      <c r="AW92" s="62"/>
     </row>
     <row r="93" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A93" s="6"/>
@@ -4876,167 +4912,356 @@
       <c r="C93" s="6"/>
       <c r="D93" s="6"/>
       <c r="E93" s="6"/>
-      <c r="AO93" s="93" t="s">
-        <v>150</v>
-      </c>
-      <c r="AP93" s="94">
-        <v>17</v>
-      </c>
-      <c r="AQ93" s="94">
-        <v>30</v>
-      </c>
-      <c r="AR93" s="94" t="s">
-        <v>379</v>
-      </c>
-      <c r="AS93" s="94" t="s">
-        <v>285</v>
-      </c>
-      <c r="AT93" s="94" t="s">
-        <v>59</v>
-      </c>
-      <c r="AU93" s="94" t="s">
-        <v>394</v>
-      </c>
-      <c r="AV93" s="94" t="s">
-        <v>387</v>
-      </c>
-      <c r="AW93" s="95" t="s">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="94" spans="1:49" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AO93" t="s">
+        <v>114</v>
+      </c>
+      <c r="AP93" s="14">
+        <v>138</v>
+      </c>
+      <c r="AR93" s="62"/>
+      <c r="AS93" s="62"/>
+      <c r="AT93" s="62"/>
+      <c r="AU93" s="62"/>
+      <c r="AV93" s="62"/>
+      <c r="AW93" s="62"/>
+    </row>
+    <row r="94" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A94" s="6"/>
       <c r="B94" s="6"/>
       <c r="C94" s="6"/>
       <c r="D94" s="6"/>
       <c r="E94" s="6"/>
-      <c r="AO94" s="96" t="s">
-        <v>152</v>
-      </c>
-      <c r="AP94" s="97">
-        <v>13</v>
-      </c>
-      <c r="AQ94" s="97">
-        <v>14</v>
-      </c>
-      <c r="AR94" s="97" t="s">
-        <v>381</v>
-      </c>
-      <c r="AS94" s="97" t="s">
-        <v>382</v>
-      </c>
-      <c r="AT94" s="97" t="s">
-        <v>383</v>
-      </c>
-      <c r="AU94" s="97" t="s">
-        <v>395</v>
-      </c>
-      <c r="AV94" s="94" t="s">
-        <v>388</v>
-      </c>
-      <c r="AW94" s="98" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="95" spans="1:49" x14ac:dyDescent="0.25">
+      <c r="AO94" t="s">
+        <v>115</v>
+      </c>
+      <c r="AP94" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="95" spans="1:49" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A95" s="6"/>
       <c r="B95" s="6"/>
       <c r="C95" s="6"/>
       <c r="D95" s="6"/>
       <c r="E95" s="6"/>
-    </row>
-    <row r="96" spans="1:49" x14ac:dyDescent="0.25">
+      <c r="AO95" t="s">
+        <v>103</v>
+      </c>
+      <c r="AP95" t="s">
+        <v>117</v>
+      </c>
+      <c r="AQ95" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="96" spans="1:49" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A96" s="6"/>
       <c r="B96" s="6"/>
       <c r="C96" s="6"/>
       <c r="D96" s="6"/>
       <c r="E96" s="6"/>
-    </row>
-    <row r="97" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="AO96" s="63" t="s">
+        <v>94</v>
+      </c>
+      <c r="AP96" s="64" t="s">
+        <v>95</v>
+      </c>
+      <c r="AQ96" s="64" t="s">
+        <v>96</v>
+      </c>
+      <c r="AR96" s="64" t="s">
+        <v>103</v>
+      </c>
+      <c r="AS96" s="64" t="s">
+        <v>102</v>
+      </c>
+      <c r="AT96" s="64" t="s">
+        <v>104</v>
+      </c>
+      <c r="AU96" s="64" t="s">
+        <v>101</v>
+      </c>
+      <c r="AV96" s="64" t="s">
+        <v>43</v>
+      </c>
+      <c r="AW96" s="65" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="97" spans="2:49" x14ac:dyDescent="0.25">
       <c r="B97" s="6"/>
       <c r="C97" s="6"/>
       <c r="D97" s="6"/>
       <c r="E97" s="6"/>
-    </row>
-    <row r="98" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="AO97" s="81" t="s">
+        <v>153</v>
+      </c>
+      <c r="AP97" s="82">
+        <v>24</v>
+      </c>
+      <c r="AQ97" s="82">
+        <v>30</v>
+      </c>
+      <c r="AR97" s="82" t="s">
+        <v>307</v>
+      </c>
+      <c r="AS97" s="82" t="s">
+        <v>277</v>
+      </c>
+      <c r="AT97" s="82" t="s">
+        <v>59</v>
+      </c>
+      <c r="AU97" s="82" t="s">
+        <v>260</v>
+      </c>
+      <c r="AV97" s="82" t="s">
+        <v>377</v>
+      </c>
+      <c r="AW97" s="83" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="98" spans="2:49" x14ac:dyDescent="0.25">
       <c r="B98" s="6"/>
       <c r="C98" s="6"/>
       <c r="D98" s="6"/>
       <c r="E98" s="6"/>
-    </row>
-    <row r="99" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="AO98" s="84" t="s">
+        <v>154</v>
+      </c>
+      <c r="AP98" s="85">
+        <v>23</v>
+      </c>
+      <c r="AQ98" s="85">
+        <v>30</v>
+      </c>
+      <c r="AR98" s="85" t="s">
+        <v>363</v>
+      </c>
+      <c r="AS98" s="85" t="s">
+        <v>277</v>
+      </c>
+      <c r="AT98" s="85" t="s">
+        <v>59</v>
+      </c>
+      <c r="AU98" s="85" t="s">
+        <v>382</v>
+      </c>
+      <c r="AV98" s="85" t="s">
+        <v>381</v>
+      </c>
+      <c r="AW98" s="86" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="99" spans="2:49" x14ac:dyDescent="0.25">
       <c r="B99" s="6"/>
       <c r="C99" s="6"/>
       <c r="D99" s="6"/>
       <c r="E99" s="6"/>
-    </row>
-    <row r="100" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="AO99" s="84" t="s">
+        <v>149</v>
+      </c>
+      <c r="AP99" s="85">
+        <v>23</v>
+      </c>
+      <c r="AQ99" s="85">
+        <v>30</v>
+      </c>
+      <c r="AR99" s="85" t="s">
+        <v>365</v>
+      </c>
+      <c r="AS99" s="85" t="s">
+        <v>277</v>
+      </c>
+      <c r="AT99" s="85" t="s">
+        <v>59</v>
+      </c>
+      <c r="AU99" s="85" t="s">
+        <v>383</v>
+      </c>
+      <c r="AV99" s="85" t="s">
+        <v>364</v>
+      </c>
+      <c r="AW99" s="86" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="100" spans="2:49" x14ac:dyDescent="0.25">
       <c r="B100" s="6"/>
       <c r="C100" s="6"/>
       <c r="D100" s="6"/>
       <c r="E100" s="6"/>
-    </row>
-    <row r="101" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="AO100" s="84" t="s">
+        <v>151</v>
+      </c>
+      <c r="AP100" s="85">
+        <v>20</v>
+      </c>
+      <c r="AQ100" s="85">
+        <v>30</v>
+      </c>
+      <c r="AR100" s="85" t="s">
+        <v>367</v>
+      </c>
+      <c r="AS100" s="85" t="s">
+        <v>277</v>
+      </c>
+      <c r="AT100" s="85" t="s">
+        <v>59</v>
+      </c>
+      <c r="AU100" s="85" t="s">
+        <v>384</v>
+      </c>
+      <c r="AV100" s="85" t="s">
+        <v>365</v>
+      </c>
+      <c r="AW100" s="86" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="101" spans="2:49" x14ac:dyDescent="0.25">
       <c r="B101" s="6"/>
       <c r="C101" s="6"/>
       <c r="D101" s="6"/>
       <c r="E101" s="6"/>
-    </row>
-    <row r="102" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="AO101" s="84" t="s">
+        <v>281</v>
+      </c>
+      <c r="AP101" s="85">
+        <v>18</v>
+      </c>
+      <c r="AQ101" s="85">
+        <v>30</v>
+      </c>
+      <c r="AR101" s="85" t="s">
+        <v>369</v>
+      </c>
+      <c r="AS101" s="85" t="s">
+        <v>277</v>
+      </c>
+      <c r="AT101" s="85" t="s">
+        <v>59</v>
+      </c>
+      <c r="AU101" s="85" t="s">
+        <v>385</v>
+      </c>
+      <c r="AV101" s="85" t="s">
+        <v>378</v>
+      </c>
+      <c r="AW101" s="86" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="102" spans="2:49" x14ac:dyDescent="0.25">
       <c r="B102" s="6"/>
       <c r="C102" s="6"/>
       <c r="D102" s="6"/>
       <c r="E102" s="6"/>
-    </row>
-    <row r="103" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="AO102" s="84" t="s">
+        <v>150</v>
+      </c>
+      <c r="AP102" s="85">
+        <v>17</v>
+      </c>
+      <c r="AQ102" s="85">
+        <v>30</v>
+      </c>
+      <c r="AR102" s="85" t="s">
+        <v>371</v>
+      </c>
+      <c r="AS102" s="85" t="s">
+        <v>277</v>
+      </c>
+      <c r="AT102" s="85" t="s">
+        <v>59</v>
+      </c>
+      <c r="AU102" s="85" t="s">
+        <v>386</v>
+      </c>
+      <c r="AV102" s="85" t="s">
+        <v>379</v>
+      </c>
+      <c r="AW102" s="86" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="103" spans="2:49" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B103" s="6"/>
       <c r="C103" s="6"/>
       <c r="D103" s="6"/>
       <c r="E103" s="6"/>
-    </row>
-    <row r="104" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="AO103" s="87" t="s">
+        <v>152</v>
+      </c>
+      <c r="AP103" s="88">
+        <v>13</v>
+      </c>
+      <c r="AQ103" s="88">
+        <v>14</v>
+      </c>
+      <c r="AR103" s="88" t="s">
+        <v>373</v>
+      </c>
+      <c r="AS103" s="88" t="s">
+        <v>374</v>
+      </c>
+      <c r="AT103" s="88" t="s">
+        <v>375</v>
+      </c>
+      <c r="AU103" s="88" t="s">
+        <v>387</v>
+      </c>
+      <c r="AV103" s="85" t="s">
+        <v>380</v>
+      </c>
+      <c r="AW103" s="89" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="104" spans="2:49" x14ac:dyDescent="0.25">
       <c r="B104" s="6"/>
       <c r="C104" s="6"/>
       <c r="D104" s="6"/>
       <c r="E104" s="6"/>
     </row>
-    <row r="105" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="105" spans="2:49" x14ac:dyDescent="0.25">
       <c r="B105" s="6"/>
       <c r="C105" s="6"/>
       <c r="D105" s="6"/>
       <c r="E105" s="6"/>
     </row>
-    <row r="106" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="106" spans="2:49" x14ac:dyDescent="0.25">
       <c r="B106" s="6"/>
       <c r="C106" s="6"/>
       <c r="D106" s="6"/>
       <c r="E106" s="6"/>
     </row>
-    <row r="107" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="107" spans="2:49" x14ac:dyDescent="0.25">
       <c r="B107" s="6"/>
       <c r="C107" s="6"/>
       <c r="D107" s="6"/>
       <c r="E107" s="6"/>
     </row>
-    <row r="108" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="108" spans="2:49" x14ac:dyDescent="0.25">
       <c r="B108" s="6"/>
       <c r="C108" s="6"/>
       <c r="D108" s="6"/>
       <c r="E108" s="6"/>
     </row>
-    <row r="109" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="109" spans="2:49" x14ac:dyDescent="0.25">
       <c r="B109" s="6"/>
       <c r="C109" s="6"/>
       <c r="D109" s="6"/>
       <c r="E109" s="6"/>
     </row>
-    <row r="110" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="110" spans="2:49" x14ac:dyDescent="0.25">
       <c r="B110" s="6"/>
       <c r="C110" s="6"/>
       <c r="D110" s="6"/>
       <c r="E110" s="6"/>
     </row>
-    <row r="111" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="111" spans="2:49" x14ac:dyDescent="0.25">
       <c r="B111" s="6"/>
       <c r="C111" s="6"/>
       <c r="D111" s="6"/>
@@ -5087,69 +5312,69 @@
     <row r="3" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="19"/>
-      <c r="B4" s="79" t="s">
+      <c r="B4" s="93" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="80"/>
-      <c r="D4" s="80"/>
-      <c r="E4" s="81"/>
-      <c r="F4" s="79" t="s">
+      <c r="C4" s="94"/>
+      <c r="D4" s="94"/>
+      <c r="E4" s="95"/>
+      <c r="F4" s="93" t="s">
         <v>24</v>
       </c>
-      <c r="G4" s="80"/>
-      <c r="H4" s="80"/>
-      <c r="I4" s="81"/>
-      <c r="J4" s="79" t="s">
+      <c r="G4" s="94"/>
+      <c r="H4" s="94"/>
+      <c r="I4" s="95"/>
+      <c r="J4" s="93" t="s">
         <v>26</v>
       </c>
-      <c r="K4" s="80"/>
-      <c r="L4" s="80"/>
-      <c r="M4" s="80"/>
-      <c r="N4" s="79" t="s">
+      <c r="K4" s="94"/>
+      <c r="L4" s="94"/>
+      <c r="M4" s="94"/>
+      <c r="N4" s="93" t="s">
         <v>27</v>
       </c>
-      <c r="O4" s="80"/>
-      <c r="P4" s="80"/>
-      <c r="Q4" s="81"/>
-      <c r="R4" s="79" t="s">
+      <c r="O4" s="94"/>
+      <c r="P4" s="94"/>
+      <c r="Q4" s="95"/>
+      <c r="R4" s="93" t="s">
         <v>25</v>
       </c>
-      <c r="S4" s="80"/>
-      <c r="T4" s="80"/>
-      <c r="U4" s="81"/>
+      <c r="S4" s="94"/>
+      <c r="T4" s="94"/>
+      <c r="U4" s="95"/>
     </row>
     <row r="5" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="20"/>
-      <c r="B5" s="82" t="s">
+      <c r="B5" s="90" t="s">
         <v>82</v>
       </c>
-      <c r="C5" s="83"/>
-      <c r="D5" s="83"/>
-      <c r="E5" s="84"/>
-      <c r="F5" s="82" t="s">
+      <c r="C5" s="91"/>
+      <c r="D5" s="91"/>
+      <c r="E5" s="92"/>
+      <c r="F5" s="90" t="s">
         <v>82</v>
       </c>
-      <c r="G5" s="83"/>
-      <c r="H5" s="83"/>
-      <c r="I5" s="84"/>
-      <c r="J5" s="82" t="s">
+      <c r="G5" s="91"/>
+      <c r="H5" s="91"/>
+      <c r="I5" s="92"/>
+      <c r="J5" s="90" t="s">
         <v>82</v>
       </c>
-      <c r="K5" s="83"/>
-      <c r="L5" s="83"/>
-      <c r="M5" s="83"/>
-      <c r="N5" s="82" t="s">
+      <c r="K5" s="91"/>
+      <c r="L5" s="91"/>
+      <c r="M5" s="91"/>
+      <c r="N5" s="90" t="s">
         <v>82</v>
       </c>
-      <c r="O5" s="83"/>
-      <c r="P5" s="83"/>
-      <c r="Q5" s="84"/>
-      <c r="R5" s="82" t="s">
+      <c r="O5" s="91"/>
+      <c r="P5" s="91"/>
+      <c r="Q5" s="92"/>
+      <c r="R5" s="90" t="s">
         <v>82</v>
       </c>
-      <c r="S5" s="83"/>
-      <c r="T5" s="83"/>
-      <c r="U5" s="84"/>
+      <c r="S5" s="91"/>
+      <c r="T5" s="91"/>
+      <c r="U5" s="92"/>
     </row>
     <row r="6" spans="1:21" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="22" t="s">
@@ -5762,62 +5987,62 @@
     </row>
     <row r="15" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="21"/>
-      <c r="B15" s="76">
+      <c r="B15" s="96">
         <f>B14+C14+D14+E14</f>
         <v>579</v>
       </c>
-      <c r="C15" s="77"/>
-      <c r="D15" s="77"/>
-      <c r="E15" s="78"/>
-      <c r="F15" s="76">
+      <c r="C15" s="97"/>
+      <c r="D15" s="97"/>
+      <c r="E15" s="98"/>
+      <c r="F15" s="96">
         <f>F14+G14+H14+I14</f>
         <v>585</v>
       </c>
-      <c r="G15" s="77"/>
-      <c r="H15" s="77"/>
-      <c r="I15" s="78"/>
-      <c r="J15" s="76">
+      <c r="G15" s="97"/>
+      <c r="H15" s="97"/>
+      <c r="I15" s="98"/>
+      <c r="J15" s="96">
         <f>J14+K14+L14+M14</f>
         <v>580</v>
       </c>
-      <c r="K15" s="77"/>
-      <c r="L15" s="77"/>
-      <c r="M15" s="77"/>
-      <c r="N15" s="76">
+      <c r="K15" s="97"/>
+      <c r="L15" s="97"/>
+      <c r="M15" s="97"/>
+      <c r="N15" s="96">
         <f>N14+O14+P14+Q14</f>
         <v>590</v>
       </c>
-      <c r="O15" s="77"/>
-      <c r="P15" s="77"/>
-      <c r="Q15" s="78"/>
-      <c r="R15" s="76">
+      <c r="O15" s="97"/>
+      <c r="P15" s="97"/>
+      <c r="Q15" s="98"/>
+      <c r="R15" s="96">
         <f>R14+S14+T14+U14</f>
         <v>571</v>
       </c>
-      <c r="S15" s="77"/>
-      <c r="T15" s="77"/>
-      <c r="U15" s="78"/>
+      <c r="S15" s="97"/>
+      <c r="T15" s="97"/>
+      <c r="U15" s="98"/>
     </row>
     <row r="20" spans="12:12" x14ac:dyDescent="0.25">
       <c r="L20" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="B15:E15"/>
+    <mergeCell ref="F15:I15"/>
+    <mergeCell ref="J15:M15"/>
+    <mergeCell ref="N15:Q15"/>
+    <mergeCell ref="R15:U15"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="F4:I4"/>
+    <mergeCell ref="J4:M4"/>
+    <mergeCell ref="N4:Q4"/>
+    <mergeCell ref="R4:U4"/>
     <mergeCell ref="B5:E5"/>
     <mergeCell ref="F5:I5"/>
     <mergeCell ref="J5:M5"/>
     <mergeCell ref="N5:Q5"/>
     <mergeCell ref="R5:U5"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="F4:I4"/>
-    <mergeCell ref="J4:M4"/>
-    <mergeCell ref="N4:Q4"/>
-    <mergeCell ref="R4:U4"/>
-    <mergeCell ref="B15:E15"/>
-    <mergeCell ref="F15:I15"/>
-    <mergeCell ref="J15:M15"/>
-    <mergeCell ref="N15:Q15"/>
-    <mergeCell ref="R15:U15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -5829,7 +6054,7 @@
   <dimension ref="A2:L26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5841,12 +6066,12 @@
   <sheetData>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D2" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -5861,7 +6086,7 @@
       <c r="G5" s="53"/>
       <c r="H5" s="54"/>
       <c r="K5" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
@@ -5888,7 +6113,7 @@
         <v>162</v>
       </c>
       <c r="K6" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -5915,10 +6140,10 @@
         <v>151</v>
       </c>
       <c r="K7" t="s">
-        <v>202</v>
+        <v>194</v>
       </c>
       <c r="L7" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
@@ -5947,10 +6172,10 @@
         <v>179</v>
       </c>
       <c r="K8" s="59" t="s">
-        <v>203</v>
+        <v>195</v>
       </c>
       <c r="L8" s="59" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -5979,10 +6204,10 @@
         <v>179</v>
       </c>
       <c r="K9" s="59" t="s">
+        <v>196</v>
+      </c>
+      <c r="L9" s="59" t="s">
         <v>204</v>
-      </c>
-      <c r="L9" s="59" t="s">
-        <v>212</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
@@ -6011,10 +6236,10 @@
         <v>179</v>
       </c>
       <c r="K10" s="59" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
       <c r="L10" s="59" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -6043,10 +6268,10 @@
         <v>179</v>
       </c>
       <c r="K11" s="59" t="s">
-        <v>206</v>
+        <v>198</v>
       </c>
       <c r="L11" s="59" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
@@ -6075,10 +6300,10 @@
         <v>179</v>
       </c>
       <c r="K12" s="59" t="s">
-        <v>207</v>
+        <v>199</v>
       </c>
       <c r="L12" s="59" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
@@ -6135,10 +6360,10 @@
     </row>
     <row r="17" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="B17" s="55" t="s">
-        <v>185</v>
+        <v>388</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
@@ -6158,13 +6383,13 @@
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="9"/>
       <c r="B19" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="C19" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="D19" s="3" t="s">
         <v>188</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>189</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -6172,13 +6397,13 @@
         <v>163</v>
       </c>
       <c r="B20" s="55" t="s">
-        <v>192</v>
+        <v>390</v>
       </c>
       <c r="C20" s="55" t="s">
-        <v>194</v>
+        <v>391</v>
       </c>
       <c r="D20" s="56" t="s">
-        <v>195</v>
+        <v>393</v>
       </c>
       <c r="E20" s="50"/>
       <c r="F20" s="50"/>
@@ -6190,13 +6415,13 @@
         <v>164</v>
       </c>
       <c r="B21" s="55" t="s">
-        <v>192</v>
+        <v>390</v>
       </c>
       <c r="C21" s="55" t="s">
-        <v>194</v>
+        <v>391</v>
       </c>
       <c r="D21" s="56" t="s">
-        <v>196</v>
+        <v>393</v>
       </c>
       <c r="E21" s="50"/>
       <c r="F21" s="50"/>
@@ -6208,13 +6433,13 @@
         <v>184</v>
       </c>
       <c r="B22" s="57" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="C22" s="57" t="s">
-        <v>197</v>
+        <v>392</v>
       </c>
       <c r="D22" s="58" t="s">
-        <v>196</v>
+        <v>394</v>
       </c>
       <c r="E22" s="50"/>
       <c r="F22" s="50"/>
@@ -6224,13 +6449,13 @@
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="2"/>
       <c r="B23" s="55" t="s">
-        <v>190</v>
+        <v>389</v>
       </c>
       <c r="C23" s="55" t="s">
-        <v>190</v>
+        <v>389</v>
       </c>
       <c r="D23" s="55" t="s">
-        <v>191</v>
+        <v>389</v>
       </c>
       <c r="E23" s="50"/>
       <c r="F23" s="50"/>
@@ -6285,23 +6510,23 @@
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="19"/>
-      <c r="B1" s="79" t="s">
+      <c r="B1" s="93" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="80"/>
-      <c r="D1" s="80"/>
-      <c r="E1" s="81"/>
+      <c r="C1" s="94"/>
+      <c r="D1" s="94"/>
+      <c r="E1" s="95"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="24" t="s">
         <v>81</v>
       </c>
-      <c r="B2" s="82" t="s">
+      <c r="B2" s="90" t="s">
         <v>82</v>
       </c>
-      <c r="C2" s="83"/>
-      <c r="D2" s="83"/>
-      <c r="E2" s="84"/>
+      <c r="C2" s="91"/>
+      <c r="D2" s="91"/>
+      <c r="E2" s="92"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
@@ -6458,13 +6683,13 @@
     </row>
     <row r="12" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="21"/>
-      <c r="B12" s="76">
+      <c r="B12" s="96">
         <f>B11+C11+D11+E11</f>
         <v>322</v>
       </c>
-      <c r="C12" s="77"/>
-      <c r="D12" s="77"/>
-      <c r="E12" s="78"/>
+      <c r="C12" s="97"/>
+      <c r="D12" s="97"/>
+      <c r="E12" s="98"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">

</xml_diff>

<commit_message>
Creaion de vlans en oficinas
</commit_message>
<xml_diff>
--- a/SUBNETEO REDES.xlsx
+++ b/SUBNETEO REDES.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Documents\Universidad\Redes II\TERCER PARCIAL\Proyecto\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AstarothiXYZ\Desktop\proyecto redes\PROYECTO-REDES\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F83D3BB8-A415-4589-90AF-CCC5EA7C4562}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9630"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Resumen" sheetId="1" r:id="rId1"/>
@@ -18,10 +19,16 @@
     <sheet name="VLANS" sheetId="6" r:id="rId4"/>
     <sheet name="Honduras" sheetId="5" state="hidden" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -903,7 +910,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1286,33 +1293,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1356,6 +1336,33 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1643,11 +1650,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AW111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AH21" workbookViewId="0">
-      <selection activeCell="AL42" sqref="AL42"/>
+    <sheetView topLeftCell="AL27" workbookViewId="0">
+      <selection activeCell="AW36" sqref="AW36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1689,7 +1696,7 @@
     <col min="41" max="41" width="17.85546875" customWidth="1"/>
     <col min="42" max="42" width="17.140625" customWidth="1"/>
     <col min="43" max="43" width="15.140625" customWidth="1"/>
-    <col min="44" max="44" width="13.42578125" customWidth="1"/>
+    <col min="44" max="44" width="16.5703125" customWidth="1"/>
     <col min="45" max="45" width="9.85546875" customWidth="1"/>
     <col min="46" max="46" width="14.42578125" customWidth="1"/>
     <col min="47" max="47" width="15.5703125" customWidth="1"/>
@@ -2976,31 +2983,31 @@
       <c r="H35" s="44"/>
       <c r="I35" s="45"/>
       <c r="AN35" s="62"/>
-      <c r="AO35" s="72" t="s">
+      <c r="AO35" s="63" t="s">
         <v>94</v>
       </c>
-      <c r="AP35" s="73" t="s">
+      <c r="AP35" s="64" t="s">
         <v>95</v>
       </c>
-      <c r="AQ35" s="73" t="s">
+      <c r="AQ35" s="64" t="s">
         <v>96</v>
       </c>
-      <c r="AR35" s="73" t="s">
+      <c r="AR35" s="64" t="s">
         <v>103</v>
       </c>
-      <c r="AS35" s="73" t="s">
+      <c r="AS35" s="64" t="s">
         <v>102</v>
       </c>
-      <c r="AT35" s="73" t="s">
+      <c r="AT35" s="64" t="s">
         <v>104</v>
       </c>
-      <c r="AU35" s="73" t="s">
+      <c r="AU35" s="64" t="s">
         <v>101</v>
       </c>
-      <c r="AV35" s="73" t="s">
+      <c r="AV35" s="64" t="s">
         <v>43</v>
       </c>
-      <c r="AW35" s="74" t="s">
+      <c r="AW35" s="65" t="s">
         <v>40</v>
       </c>
     </row>
@@ -3015,31 +3022,31 @@
       <c r="H36" s="42"/>
       <c r="I36" s="42"/>
       <c r="AN36" s="62"/>
-      <c r="AO36" s="75" t="s">
+      <c r="AO36" s="66" t="s">
         <v>277</v>
       </c>
-      <c r="AP36" s="76">
+      <c r="AP36" s="67">
         <v>143</v>
       </c>
-      <c r="AQ36" s="76">
+      <c r="AQ36" s="67">
         <v>254</v>
       </c>
-      <c r="AR36" s="76" t="s">
+      <c r="AR36" s="67" t="s">
         <v>117</v>
       </c>
-      <c r="AS36" s="76" t="s">
+      <c r="AS36" s="67" t="s">
         <v>116</v>
       </c>
-      <c r="AT36" s="76" t="s">
+      <c r="AT36" s="67" t="s">
         <v>232</v>
       </c>
-      <c r="AU36" s="76" t="s">
+      <c r="AU36" s="67" t="s">
         <v>235</v>
       </c>
-      <c r="AV36" s="76" t="s">
+      <c r="AV36" s="67" t="s">
         <v>263</v>
       </c>
-      <c r="AW36" s="77" t="s">
+      <c r="AW36" s="68" t="s">
         <v>267</v>
       </c>
     </row>
@@ -3053,31 +3060,31 @@
       <c r="G37" s="42"/>
       <c r="H37" s="42"/>
       <c r="I37" s="42"/>
-      <c r="AO37" s="75" t="s">
+      <c r="AO37" s="66" t="s">
         <v>278</v>
       </c>
-      <c r="AP37" s="76">
+      <c r="AP37" s="67">
         <v>50</v>
       </c>
-      <c r="AQ37" s="76">
+      <c r="AQ37" s="67">
         <v>62</v>
       </c>
-      <c r="AR37" s="76" t="s">
+      <c r="AR37" s="67" t="s">
         <v>280</v>
       </c>
-      <c r="AS37" s="76" t="s">
+      <c r="AS37" s="67" t="s">
         <v>279</v>
       </c>
-      <c r="AT37" s="76" t="s">
+      <c r="AT37" s="67" t="s">
         <v>258</v>
       </c>
-      <c r="AU37" s="76" t="s">
+      <c r="AU37" s="67" t="s">
         <v>287</v>
       </c>
-      <c r="AV37" s="76" t="s">
+      <c r="AV37" s="67" t="s">
         <v>285</v>
       </c>
-      <c r="AW37" s="77" t="s">
+      <c r="AW37" s="68" t="s">
         <v>281</v>
       </c>
     </row>
@@ -3091,32 +3098,32 @@
       <c r="G38" s="42"/>
       <c r="H38" s="42"/>
       <c r="I38" s="42"/>
-      <c r="AN38" s="90"/>
-      <c r="AO38" s="78" t="s">
+      <c r="AN38" s="81"/>
+      <c r="AO38" s="69" t="s">
         <v>282</v>
       </c>
-      <c r="AP38" s="79">
+      <c r="AP38" s="70">
         <v>50</v>
       </c>
-      <c r="AQ38" s="79">
+      <c r="AQ38" s="70">
         <v>62</v>
       </c>
-      <c r="AR38" s="79" t="s">
+      <c r="AR38" s="70" t="s">
         <v>280</v>
       </c>
-      <c r="AS38" s="79" t="s">
+      <c r="AS38" s="70" t="s">
         <v>279</v>
       </c>
-      <c r="AT38" s="79" t="s">
+      <c r="AT38" s="70" t="s">
         <v>283</v>
       </c>
-      <c r="AU38" s="79" t="s">
+      <c r="AU38" s="70" t="s">
         <v>288</v>
       </c>
-      <c r="AV38" s="79" t="s">
+      <c r="AV38" s="70" t="s">
         <v>286</v>
       </c>
-      <c r="AW38" s="80" t="s">
+      <c r="AW38" s="71" t="s">
         <v>284</v>
       </c>
     </row>
@@ -3205,118 +3212,118 @@
       </c>
     </row>
     <row r="44" spans="1:49" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="AO44" s="87" t="s">
+      <c r="AO44" s="78" t="s">
         <v>94</v>
       </c>
-      <c r="AP44" s="88" t="s">
+      <c r="AP44" s="79" t="s">
         <v>95</v>
       </c>
-      <c r="AQ44" s="88" t="s">
+      <c r="AQ44" s="79" t="s">
         <v>96</v>
       </c>
-      <c r="AR44" s="88" t="s">
+      <c r="AR44" s="79" t="s">
         <v>103</v>
       </c>
-      <c r="AS44" s="88" t="s">
+      <c r="AS44" s="79" t="s">
         <v>102</v>
       </c>
-      <c r="AT44" s="88" t="s">
+      <c r="AT44" s="79" t="s">
         <v>104</v>
       </c>
-      <c r="AU44" s="88" t="s">
+      <c r="AU44" s="79" t="s">
         <v>101</v>
       </c>
-      <c r="AV44" s="88" t="s">
+      <c r="AV44" s="79" t="s">
         <v>43</v>
       </c>
-      <c r="AW44" s="89" t="s">
+      <c r="AW44" s="80" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="45" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="AO45" s="81" t="s">
+      <c r="AO45" s="72" t="s">
         <v>277</v>
       </c>
-      <c r="AP45" s="82">
+      <c r="AP45" s="73">
         <v>143</v>
       </c>
-      <c r="AQ45" s="82">
+      <c r="AQ45" s="73">
         <v>254</v>
       </c>
-      <c r="AR45" s="82" t="s">
+      <c r="AR45" s="73" t="s">
         <v>117</v>
       </c>
-      <c r="AS45" s="82" t="s">
+      <c r="AS45" s="73" t="s">
         <v>116</v>
       </c>
-      <c r="AT45" s="82" t="s">
+      <c r="AT45" s="73" t="s">
         <v>232</v>
       </c>
-      <c r="AU45" s="82" t="s">
+      <c r="AU45" s="73" t="s">
         <v>235</v>
       </c>
-      <c r="AV45" s="82" t="s">
+      <c r="AV45" s="73" t="s">
         <v>263</v>
       </c>
-      <c r="AW45" s="83" t="s">
+      <c r="AW45" s="74" t="s">
         <v>267</v>
       </c>
     </row>
     <row r="46" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="AO46" s="81" t="s">
+      <c r="AO46" s="72" t="s">
         <v>278</v>
       </c>
-      <c r="AP46" s="82">
+      <c r="AP46" s="73">
         <v>50</v>
       </c>
-      <c r="AQ46" s="82">
+      <c r="AQ46" s="73">
         <v>62</v>
       </c>
-      <c r="AR46" s="82" t="s">
+      <c r="AR46" s="73" t="s">
         <v>280</v>
       </c>
-      <c r="AS46" s="82" t="s">
+      <c r="AS46" s="73" t="s">
         <v>279</v>
       </c>
-      <c r="AT46" s="82" t="s">
+      <c r="AT46" s="73" t="s">
         <v>258</v>
       </c>
-      <c r="AU46" s="82" t="s">
+      <c r="AU46" s="73" t="s">
         <v>287</v>
       </c>
-      <c r="AV46" s="82" t="s">
+      <c r="AV46" s="73" t="s">
         <v>285</v>
       </c>
-      <c r="AW46" s="83" t="s">
+      <c r="AW46" s="74" t="s">
         <v>281</v>
       </c>
     </row>
     <row r="47" spans="1:49" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="AO47" s="84" t="s">
+      <c r="AO47" s="75" t="s">
         <v>282</v>
       </c>
-      <c r="AP47" s="85">
+      <c r="AP47" s="76">
         <v>50</v>
       </c>
-      <c r="AQ47" s="85">
+      <c r="AQ47" s="76">
         <v>62</v>
       </c>
-      <c r="AR47" s="85" t="s">
+      <c r="AR47" s="76" t="s">
         <v>280</v>
       </c>
-      <c r="AS47" s="85" t="s">
+      <c r="AS47" s="76" t="s">
         <v>279</v>
       </c>
-      <c r="AT47" s="85" t="s">
+      <c r="AT47" s="76" t="s">
         <v>283</v>
       </c>
-      <c r="AU47" s="85" t="s">
+      <c r="AU47" s="76" t="s">
         <v>288</v>
       </c>
-      <c r="AV47" s="85" t="s">
+      <c r="AV47" s="76" t="s">
         <v>286</v>
       </c>
-      <c r="AW47" s="86" t="s">
+      <c r="AW47" s="77" t="s">
         <v>284</v>
       </c>
     </row>
@@ -3805,7 +3812,7 @@
       <c r="E111" s="6"/>
     </row>
   </sheetData>
-  <sortState ref="K36:L38">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="K36:L38">
     <sortCondition ref="L36"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3814,7 +3821,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="C11:J15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3964,7 +3971,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:U20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3999,69 +4006,69 @@
     <row r="3" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="19"/>
-      <c r="B4" s="66" t="s">
+      <c r="B4" s="85" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="67"/>
-      <c r="D4" s="67"/>
-      <c r="E4" s="68"/>
-      <c r="F4" s="66" t="s">
+      <c r="C4" s="86"/>
+      <c r="D4" s="86"/>
+      <c r="E4" s="87"/>
+      <c r="F4" s="85" t="s">
         <v>24</v>
       </c>
-      <c r="G4" s="67"/>
-      <c r="H4" s="67"/>
-      <c r="I4" s="68"/>
-      <c r="J4" s="66" t="s">
+      <c r="G4" s="86"/>
+      <c r="H4" s="86"/>
+      <c r="I4" s="87"/>
+      <c r="J4" s="85" t="s">
         <v>26</v>
       </c>
-      <c r="K4" s="67"/>
-      <c r="L4" s="67"/>
-      <c r="M4" s="67"/>
-      <c r="N4" s="66" t="s">
+      <c r="K4" s="86"/>
+      <c r="L4" s="86"/>
+      <c r="M4" s="86"/>
+      <c r="N4" s="85" t="s">
         <v>27</v>
       </c>
-      <c r="O4" s="67"/>
-      <c r="P4" s="67"/>
-      <c r="Q4" s="68"/>
-      <c r="R4" s="66" t="s">
+      <c r="O4" s="86"/>
+      <c r="P4" s="86"/>
+      <c r="Q4" s="87"/>
+      <c r="R4" s="85" t="s">
         <v>25</v>
       </c>
-      <c r="S4" s="67"/>
-      <c r="T4" s="67"/>
-      <c r="U4" s="68"/>
+      <c r="S4" s="86"/>
+      <c r="T4" s="86"/>
+      <c r="U4" s="87"/>
     </row>
     <row r="5" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="20"/>
-      <c r="B5" s="63" t="s">
+      <c r="B5" s="88" t="s">
         <v>82</v>
       </c>
-      <c r="C5" s="64"/>
-      <c r="D5" s="64"/>
-      <c r="E5" s="65"/>
-      <c r="F5" s="63" t="s">
+      <c r="C5" s="89"/>
+      <c r="D5" s="89"/>
+      <c r="E5" s="90"/>
+      <c r="F5" s="88" t="s">
         <v>82</v>
       </c>
-      <c r="G5" s="64"/>
-      <c r="H5" s="64"/>
-      <c r="I5" s="65"/>
-      <c r="J5" s="63" t="s">
+      <c r="G5" s="89"/>
+      <c r="H5" s="89"/>
+      <c r="I5" s="90"/>
+      <c r="J5" s="88" t="s">
         <v>82</v>
       </c>
-      <c r="K5" s="64"/>
-      <c r="L5" s="64"/>
-      <c r="M5" s="64"/>
-      <c r="N5" s="63" t="s">
+      <c r="K5" s="89"/>
+      <c r="L5" s="89"/>
+      <c r="M5" s="89"/>
+      <c r="N5" s="88" t="s">
         <v>82</v>
       </c>
-      <c r="O5" s="64"/>
-      <c r="P5" s="64"/>
-      <c r="Q5" s="65"/>
-      <c r="R5" s="63" t="s">
+      <c r="O5" s="89"/>
+      <c r="P5" s="89"/>
+      <c r="Q5" s="90"/>
+      <c r="R5" s="88" t="s">
         <v>82</v>
       </c>
-      <c r="S5" s="64"/>
-      <c r="T5" s="64"/>
-      <c r="U5" s="65"/>
+      <c r="S5" s="89"/>
+      <c r="T5" s="89"/>
+      <c r="U5" s="90"/>
     </row>
     <row r="6" spans="1:21" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="22" t="s">
@@ -4674,62 +4681,62 @@
     </row>
     <row r="15" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="21"/>
-      <c r="B15" s="69">
+      <c r="B15" s="82">
         <f>B14+C14+D14+E14</f>
         <v>579</v>
       </c>
-      <c r="C15" s="70"/>
-      <c r="D15" s="70"/>
-      <c r="E15" s="71"/>
-      <c r="F15" s="69">
+      <c r="C15" s="83"/>
+      <c r="D15" s="83"/>
+      <c r="E15" s="84"/>
+      <c r="F15" s="82">
         <f>F14+G14+H14+I14</f>
         <v>585</v>
       </c>
-      <c r="G15" s="70"/>
-      <c r="H15" s="70"/>
-      <c r="I15" s="71"/>
-      <c r="J15" s="69">
+      <c r="G15" s="83"/>
+      <c r="H15" s="83"/>
+      <c r="I15" s="84"/>
+      <c r="J15" s="82">
         <f>J14+K14+L14+M14</f>
         <v>580</v>
       </c>
-      <c r="K15" s="70"/>
-      <c r="L15" s="70"/>
-      <c r="M15" s="70"/>
-      <c r="N15" s="69">
+      <c r="K15" s="83"/>
+      <c r="L15" s="83"/>
+      <c r="M15" s="83"/>
+      <c r="N15" s="82">
         <f>N14+O14+P14+Q14</f>
         <v>590</v>
       </c>
-      <c r="O15" s="70"/>
-      <c r="P15" s="70"/>
-      <c r="Q15" s="71"/>
-      <c r="R15" s="69">
+      <c r="O15" s="83"/>
+      <c r="P15" s="83"/>
+      <c r="Q15" s="84"/>
+      <c r="R15" s="82">
         <f>R14+S14+T14+U14</f>
         <v>571</v>
       </c>
-      <c r="S15" s="70"/>
-      <c r="T15" s="70"/>
-      <c r="U15" s="71"/>
+      <c r="S15" s="83"/>
+      <c r="T15" s="83"/>
+      <c r="U15" s="84"/>
     </row>
     <row r="20" spans="12:12" x14ac:dyDescent="0.25">
       <c r="L20" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="F5:I5"/>
+    <mergeCell ref="J5:M5"/>
+    <mergeCell ref="N5:Q5"/>
+    <mergeCell ref="R5:U5"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="F4:I4"/>
+    <mergeCell ref="J4:M4"/>
+    <mergeCell ref="N4:Q4"/>
+    <mergeCell ref="R4:U4"/>
     <mergeCell ref="B15:E15"/>
     <mergeCell ref="F15:I15"/>
     <mergeCell ref="J15:M15"/>
     <mergeCell ref="N15:Q15"/>
     <mergeCell ref="R15:U15"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="F4:I4"/>
-    <mergeCell ref="J4:M4"/>
-    <mergeCell ref="N4:Q4"/>
-    <mergeCell ref="R4:U4"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="F5:I5"/>
-    <mergeCell ref="J5:M5"/>
-    <mergeCell ref="N5:Q5"/>
-    <mergeCell ref="R5:U5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -4737,11 +4744,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A2:L26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5183,7 +5190,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:W126"/>
   <sheetViews>
     <sheetView topLeftCell="K99" workbookViewId="0">
@@ -5197,23 +5204,23 @@
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="19"/>
-      <c r="B1" s="66" t="s">
+      <c r="B1" s="85" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="67"/>
-      <c r="D1" s="67"/>
-      <c r="E1" s="68"/>
+      <c r="C1" s="86"/>
+      <c r="D1" s="86"/>
+      <c r="E1" s="87"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="24" t="s">
         <v>81</v>
       </c>
-      <c r="B2" s="63" t="s">
+      <c r="B2" s="88" t="s">
         <v>82</v>
       </c>
-      <c r="C2" s="64"/>
-      <c r="D2" s="64"/>
-      <c r="E2" s="65"/>
+      <c r="C2" s="89"/>
+      <c r="D2" s="89"/>
+      <c r="E2" s="90"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
@@ -5370,13 +5377,13 @@
     </row>
     <row r="12" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="21"/>
-      <c r="B12" s="69">
+      <c r="B12" s="82">
         <f>B11+C11+D11+E11</f>
         <v>322</v>
       </c>
-      <c r="C12" s="70"/>
-      <c r="D12" s="70"/>
-      <c r="E12" s="71"/>
+      <c r="C12" s="83"/>
+      <c r="D12" s="83"/>
+      <c r="E12" s="84"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">

</xml_diff>